<commit_message>
Added 10_01 per-country topic descrimination aug_meta generation model
</commit_message>
<xml_diff>
--- a/csv_out/country_classification/country_classification_comparison_using_grouped_words_full_updated.xlsx
+++ b/csv_out/country_classification/country_classification_comparison_using_grouped_words_full_updated.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23001"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23029"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Repos\IMF_VE_News\csv_out\new2\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Repos\IMF_VE_News\csv_out\country_classification\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66E37113-09D7-42FC-AD6E-AB1A235638CF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74D1B1C6-C86E-4B13-98D1-5AE84E4943C9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="42">
   <si>
     <t>All Other Sentiments</t>
   </si>
@@ -143,6 +143,9 @@
   </si>
   <si>
     <t>All Crisis Countries - 20 Countries from Kaminsky and Reinhart 1999</t>
+  </si>
+  <si>
+    <t>All Crisis Countries (Title + Full Document)</t>
   </si>
 </sst>
 </file>
@@ -741,7 +744,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="43">
+  <cellXfs count="40">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
@@ -754,9 +757,6 @@
     <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="33" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="164" fontId="0" fillId="35" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="35" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
@@ -766,31 +766,31 @@
     <xf numFmtId="164" fontId="0" fillId="33" borderId="12" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="33" borderId="13" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="33" borderId="14" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="35" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="35" borderId="11" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="35" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="14" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1146,113 +1146,114 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AE45"/>
+  <dimension ref="A1:AF48"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A49" sqref="A48:A49"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="71.08984375" style="5" bestFit="1" customWidth="1"/>
     <col min="2" max="31" width="10.08984375" style="5" customWidth="1"/>
-    <col min="32" max="16384" width="8.7265625" style="42"/>
+    <col min="32" max="16384" width="8.7265625" style="35"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:31" ht="26" x14ac:dyDescent="0.6">
+    <row r="1" spans="1:32" ht="26" x14ac:dyDescent="0.6">
       <c r="A1" s="4" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="3" spans="1:31" ht="21" x14ac:dyDescent="0.5">
-      <c r="A3" s="35" t="s">
+    <row r="3" spans="1:32" ht="21" x14ac:dyDescent="0.5">
+      <c r="A3" s="29" t="s">
         <v>40</v>
       </c>
-      <c r="B3" s="36"/>
-      <c r="C3" s="36"/>
-      <c r="D3" s="36"/>
-      <c r="E3" s="36"/>
-      <c r="F3" s="36"/>
-      <c r="G3" s="36"/>
-      <c r="H3" s="36"/>
-      <c r="I3" s="36"/>
-      <c r="J3" s="36"/>
-      <c r="K3" s="36"/>
-      <c r="L3" s="36"/>
-      <c r="M3" s="36"/>
-      <c r="N3" s="36"/>
-      <c r="O3" s="36"/>
-      <c r="P3" s="36"/>
-      <c r="Q3" s="36"/>
-      <c r="R3" s="36"/>
-      <c r="S3" s="36"/>
-      <c r="T3" s="36"/>
-      <c r="U3" s="36"/>
-      <c r="V3" s="36"/>
-      <c r="W3" s="36"/>
-      <c r="X3" s="36"/>
-      <c r="Y3" s="36"/>
-      <c r="Z3" s="36"/>
-      <c r="AA3" s="36"/>
-      <c r="AB3" s="36"/>
-      <c r="AC3" s="36"/>
-      <c r="AD3" s="36"/>
-      <c r="AE3" s="37"/>
-    </row>
-    <row r="4" spans="1:31" x14ac:dyDescent="0.35">
+      <c r="B3" s="30"/>
+      <c r="C3" s="30"/>
+      <c r="D3" s="30"/>
+      <c r="E3" s="30"/>
+      <c r="F3" s="30"/>
+      <c r="G3" s="30"/>
+      <c r="H3" s="30"/>
+      <c r="I3" s="30"/>
+      <c r="J3" s="30"/>
+      <c r="K3" s="30"/>
+      <c r="L3" s="30"/>
+      <c r="M3" s="30"/>
+      <c r="N3" s="30"/>
+      <c r="O3" s="30"/>
+      <c r="P3" s="30"/>
+      <c r="Q3" s="30"/>
+      <c r="R3" s="30"/>
+      <c r="S3" s="30"/>
+      <c r="T3" s="30"/>
+      <c r="U3" s="30"/>
+      <c r="V3" s="30"/>
+      <c r="W3" s="30"/>
+      <c r="X3" s="30"/>
+      <c r="Y3" s="30"/>
+      <c r="Z3" s="30"/>
+      <c r="AA3" s="30"/>
+      <c r="AB3" s="30"/>
+      <c r="AC3" s="30"/>
+      <c r="AD3" s="30"/>
+      <c r="AE3" s="31"/>
+    </row>
+    <row r="4" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A4" s="3"/>
-      <c r="B4" s="34" t="s">
+      <c r="B4" s="36" t="s">
         <v>0</v>
       </c>
-      <c r="C4" s="12"/>
-      <c r="D4" s="31"/>
-      <c r="E4" s="34" t="s">
+      <c r="C4" s="37"/>
+      <c r="D4" s="38"/>
+      <c r="E4" s="36" t="s">
         <v>4</v>
       </c>
-      <c r="F4" s="12"/>
-      <c r="G4" s="31"/>
-      <c r="H4" s="34" t="s">
+      <c r="F4" s="37"/>
+      <c r="G4" s="38"/>
+      <c r="H4" s="36" t="s">
         <v>5</v>
       </c>
-      <c r="I4" s="12"/>
-      <c r="J4" s="31"/>
-      <c r="K4" s="34" t="s">
+      <c r="I4" s="37"/>
+      <c r="J4" s="38"/>
+      <c r="K4" s="36" t="s">
         <v>6</v>
       </c>
-      <c r="L4" s="12"/>
-      <c r="M4" s="31"/>
-      <c r="N4" s="34" t="s">
+      <c r="L4" s="37"/>
+      <c r="M4" s="38"/>
+      <c r="N4" s="36" t="s">
         <v>7</v>
       </c>
-      <c r="O4" s="12"/>
-      <c r="P4" s="31"/>
-      <c r="Q4" s="34" t="s">
+      <c r="O4" s="37"/>
+      <c r="P4" s="38"/>
+      <c r="Q4" s="36" t="s">
         <v>8</v>
       </c>
-      <c r="R4" s="12"/>
-      <c r="S4" s="31"/>
-      <c r="T4" s="34" t="s">
+      <c r="R4" s="37"/>
+      <c r="S4" s="38"/>
+      <c r="T4" s="36" t="s">
         <v>9</v>
       </c>
-      <c r="U4" s="12"/>
-      <c r="V4" s="31"/>
-      <c r="W4" s="34" t="s">
+      <c r="U4" s="37"/>
+      <c r="V4" s="38"/>
+      <c r="W4" s="36" t="s">
         <v>10</v>
       </c>
-      <c r="X4" s="12"/>
-      <c r="Y4" s="31"/>
-      <c r="Z4" s="34" t="s">
+      <c r="X4" s="37"/>
+      <c r="Y4" s="38"/>
+      <c r="Z4" s="36" t="s">
         <v>11</v>
       </c>
-      <c r="AA4" s="12"/>
-      <c r="AB4" s="31"/>
-      <c r="AC4" s="34" t="s">
+      <c r="AA4" s="37"/>
+      <c r="AB4" s="38"/>
+      <c r="AC4" s="36" t="s">
         <v>12</v>
       </c>
-      <c r="AD4" s="12"/>
-      <c r="AE4" s="31"/>
-    </row>
-    <row r="5" spans="1:31" x14ac:dyDescent="0.35">
+      <c r="AD4" s="37"/>
+      <c r="AE4" s="38"/>
+      <c r="AF4" s="39"/>
+    </row>
+    <row r="5" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A5" s="3" t="s">
         <v>13</v>
       </c>
@@ -1262,7 +1263,7 @@
       <c r="C5" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="D5" s="32" t="s">
+      <c r="D5" s="28" t="s">
         <v>1</v>
       </c>
       <c r="E5" s="3" t="s">
@@ -1271,7 +1272,7 @@
       <c r="F5" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="G5" s="32" t="s">
+      <c r="G5" s="28" t="s">
         <v>1</v>
       </c>
       <c r="H5" s="3" t="s">
@@ -1280,7 +1281,7 @@
       <c r="I5" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="J5" s="32" t="s">
+      <c r="J5" s="28" t="s">
         <v>1</v>
       </c>
       <c r="K5" s="3" t="s">
@@ -1289,7 +1290,7 @@
       <c r="L5" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="M5" s="32" t="s">
+      <c r="M5" s="28" t="s">
         <v>1</v>
       </c>
       <c r="N5" s="3" t="s">
@@ -1298,7 +1299,7 @@
       <c r="O5" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="P5" s="32" t="s">
+      <c r="P5" s="28" t="s">
         <v>1</v>
       </c>
       <c r="Q5" s="3" t="s">
@@ -1307,7 +1308,7 @@
       <c r="R5" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="S5" s="32" t="s">
+      <c r="S5" s="28" t="s">
         <v>1</v>
       </c>
       <c r="T5" s="3" t="s">
@@ -1316,7 +1317,7 @@
       <c r="U5" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="V5" s="32" t="s">
+      <c r="V5" s="28" t="s">
         <v>1</v>
       </c>
       <c r="W5" s="3" t="s">
@@ -1325,7 +1326,7 @@
       <c r="X5" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="Y5" s="32" t="s">
+      <c r="Y5" s="28" t="s">
         <v>1</v>
       </c>
       <c r="Z5" s="3" t="s">
@@ -1334,7 +1335,7 @@
       <c r="AA5" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="AB5" s="32" t="s">
+      <c r="AB5" s="28" t="s">
         <v>1</v>
       </c>
       <c r="AC5" s="3" t="s">
@@ -1343,141 +1344,144 @@
       <c r="AD5" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="AE5" s="32" t="s">
+      <c r="AE5" s="28" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="6" spans="1:31" x14ac:dyDescent="0.35">
-      <c r="A6" s="17" t="s">
+      <c r="AF5" s="39"/>
+    </row>
+    <row r="6" spans="1:32" x14ac:dyDescent="0.35">
+      <c r="A6" s="16" t="s">
         <v>14</v>
       </c>
-      <c r="B6" s="17"/>
-      <c r="C6" s="18"/>
-      <c r="D6" s="41"/>
-      <c r="E6" s="17"/>
-      <c r="F6" s="18"/>
-      <c r="G6" s="41"/>
-      <c r="H6" s="17"/>
-      <c r="I6" s="18"/>
-      <c r="J6" s="41"/>
-      <c r="K6" s="17"/>
-      <c r="L6" s="18"/>
-      <c r="M6" s="41"/>
-      <c r="N6" s="17"/>
-      <c r="O6" s="18"/>
-      <c r="P6" s="41"/>
-      <c r="Q6" s="17"/>
-      <c r="R6" s="18"/>
-      <c r="S6" s="41"/>
-      <c r="T6" s="17"/>
-      <c r="U6" s="18"/>
-      <c r="V6" s="41"/>
-      <c r="W6" s="17"/>
-      <c r="X6" s="18"/>
-      <c r="Y6" s="41"/>
-      <c r="Z6" s="17"/>
-      <c r="AA6" s="18"/>
-      <c r="AB6" s="41"/>
-      <c r="AC6" s="17"/>
-      <c r="AD6" s="18"/>
-      <c r="AE6" s="41"/>
-    </row>
-    <row r="7" spans="1:31" x14ac:dyDescent="0.35">
-      <c r="A7" s="16" t="s">
+      <c r="B6" s="16"/>
+      <c r="C6" s="17"/>
+      <c r="D6" s="34"/>
+      <c r="E6" s="16"/>
+      <c r="F6" s="17"/>
+      <c r="G6" s="34"/>
+      <c r="H6" s="16"/>
+      <c r="I6" s="17"/>
+      <c r="J6" s="34"/>
+      <c r="K6" s="16"/>
+      <c r="L6" s="17"/>
+      <c r="M6" s="34"/>
+      <c r="N6" s="16"/>
+      <c r="O6" s="17"/>
+      <c r="P6" s="34"/>
+      <c r="Q6" s="16"/>
+      <c r="R6" s="17"/>
+      <c r="S6" s="34"/>
+      <c r="T6" s="16"/>
+      <c r="U6" s="17"/>
+      <c r="V6" s="34"/>
+      <c r="W6" s="16"/>
+      <c r="X6" s="17"/>
+      <c r="Y6" s="34"/>
+      <c r="Z6" s="16"/>
+      <c r="AA6" s="17"/>
+      <c r="AB6" s="34"/>
+      <c r="AC6" s="16"/>
+      <c r="AD6" s="17"/>
+      <c r="AE6" s="34"/>
+      <c r="AF6" s="39"/>
+    </row>
+    <row r="7" spans="1:32" x14ac:dyDescent="0.35">
+      <c r="A7" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="B7" s="14">
+      <c r="B7" s="13">
         <v>0.51454138702460805</v>
       </c>
-      <c r="C7" s="15">
+      <c r="C7" s="14">
         <v>0.206278026905829</v>
       </c>
-      <c r="D7" s="23">
+      <c r="D7" s="21">
         <v>0.82142857142857095</v>
       </c>
-      <c r="E7" s="14">
+      <c r="E7" s="13">
         <v>0.53097345132743301</v>
       </c>
-      <c r="F7" s="15">
+      <c r="F7" s="14">
         <v>0.218181818181818</v>
       </c>
-      <c r="G7" s="23">
+      <c r="G7" s="21">
         <v>0.82758620689655105</v>
       </c>
-      <c r="H7" s="14">
+      <c r="H7" s="13">
         <v>0.51569506726457304</v>
       </c>
-      <c r="I7" s="15">
+      <c r="I7" s="14">
         <v>0.20720720720720701</v>
       </c>
-      <c r="J7" s="23">
+      <c r="J7" s="21">
         <v>0.82142857142857095</v>
       </c>
-      <c r="K7" s="14">
+      <c r="K7" s="13">
         <v>0.44973544973544899</v>
       </c>
-      <c r="L7" s="15">
+      <c r="L7" s="14">
         <v>0.155963302752293</v>
       </c>
-      <c r="M7" s="23">
+      <c r="M7" s="21">
         <v>0.85</v>
       </c>
-      <c r="N7" s="14">
+      <c r="N7" s="13">
         <v>0.44025157232704398</v>
       </c>
-      <c r="O7" s="15">
+      <c r="O7" s="14">
         <v>0.15384615384615299</v>
       </c>
-      <c r="P7" s="23">
+      <c r="P7" s="21">
         <v>0.82352941176470495</v>
       </c>
-      <c r="Q7" s="14">
+      <c r="Q7" s="13">
         <v>0.48693586698337199</v>
       </c>
-      <c r="R7" s="15">
+      <c r="R7" s="14">
         <v>0.18222222222222201</v>
       </c>
-      <c r="S7" s="23">
+      <c r="S7" s="21">
         <v>0.83673469387755095</v>
       </c>
-      <c r="T7" s="14">
+      <c r="T7" s="13">
         <v>0.54766734279918805</v>
       </c>
-      <c r="U7" s="15">
+      <c r="U7" s="14">
         <v>0.21686746987951799</v>
       </c>
-      <c r="V7" s="23">
+      <c r="V7" s="21">
         <v>0.88524590163934402</v>
       </c>
-      <c r="W7" s="14">
+      <c r="W7" s="13">
         <v>0.53470919324577804</v>
       </c>
-      <c r="X7" s="15">
+      <c r="X7" s="14">
         <v>0.20577617328519801</v>
       </c>
-      <c r="Y7" s="23">
+      <c r="Y7" s="21">
         <v>0.890625</v>
       </c>
-      <c r="Z7" s="14">
+      <c r="Z7" s="13">
         <v>0.50223214285714202</v>
       </c>
-      <c r="AA7" s="15">
+      <c r="AA7" s="14">
         <v>0.197368421052631</v>
       </c>
-      <c r="AB7" s="23">
+      <c r="AB7" s="21">
         <v>0.81818181818181801</v>
       </c>
-      <c r="AC7" s="14">
+      <c r="AC7" s="13">
         <v>0.473977695167286</v>
       </c>
-      <c r="AD7" s="15">
+      <c r="AD7" s="14">
         <v>0.17346938775510201</v>
       </c>
-      <c r="AE7" s="23">
+      <c r="AE7" s="21">
         <v>0.83606557377049096</v>
       </c>
-    </row>
-    <row r="8" spans="1:31" x14ac:dyDescent="0.35">
+      <c r="AF7" s="39"/>
+    </row>
+    <row r="8" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A8" s="3" t="s">
         <v>16</v>
       </c>
@@ -1487,7 +1491,7 @@
       <c r="C8" s="10">
         <v>0.15</v>
       </c>
-      <c r="D8" s="24">
+      <c r="D8" s="22">
         <v>0.56756756756756699</v>
       </c>
       <c r="E8" s="6">
@@ -1496,7 +1500,7 @@
       <c r="F8" s="10">
         <v>0.127516778523489</v>
       </c>
-      <c r="G8" s="24">
+      <c r="G8" s="22">
         <v>0.52777777777777701</v>
       </c>
       <c r="H8" s="6">
@@ -1505,7 +1509,7 @@
       <c r="I8" s="10">
         <v>0.118055555555555</v>
       </c>
-      <c r="J8" s="24">
+      <c r="J8" s="22">
         <v>0.5</v>
       </c>
       <c r="K8" s="6">
@@ -1514,7 +1518,7 @@
       <c r="L8" s="10">
         <v>0.16140350877192899</v>
       </c>
-      <c r="M8" s="24">
+      <c r="M8" s="22">
         <v>0.80701754385964897</v>
       </c>
       <c r="N8" s="6">
@@ -1523,7 +1527,7 @@
       <c r="O8" s="10">
         <v>0.14150943396226401</v>
       </c>
-      <c r="P8" s="24">
+      <c r="P8" s="22">
         <v>0.73170731707317005</v>
       </c>
       <c r="Q8" s="6">
@@ -1532,7 +1536,7 @@
       <c r="R8" s="10">
         <v>0.105263157894736</v>
       </c>
-      <c r="S8" s="24">
+      <c r="S8" s="22">
         <v>0.47058823529411697</v>
       </c>
       <c r="T8" s="6">
@@ -1541,7 +1545,7 @@
       <c r="U8" s="10">
         <v>0.13483146067415699</v>
       </c>
-      <c r="V8" s="24">
+      <c r="V8" s="22">
         <v>0.63157894736842102</v>
       </c>
       <c r="W8" s="6">
@@ -1550,7 +1554,7 @@
       <c r="X8" s="10">
         <v>0.14285714285714199</v>
       </c>
-      <c r="Y8" s="24">
+      <c r="Y8" s="22">
         <v>0.69230769230769196</v>
       </c>
       <c r="Z8" s="6">
@@ -1559,7 +1563,7 @@
       <c r="AA8" s="10">
         <v>0.13772455089820301</v>
       </c>
-      <c r="AB8" s="24">
+      <c r="AB8" s="22">
         <v>0.60526315789473595</v>
       </c>
       <c r="AC8" s="6">
@@ -1568,2427 +1572,2590 @@
       <c r="AD8" s="10">
         <v>0.12807881773398999</v>
       </c>
-      <c r="AE8" s="24">
+      <c r="AE8" s="22">
         <v>0.66666666666666596</v>
       </c>
-    </row>
-    <row r="9" spans="1:31" x14ac:dyDescent="0.35">
-      <c r="A9" s="3"/>
+      <c r="AF8" s="39"/>
+    </row>
+    <row r="9" spans="1:32" x14ac:dyDescent="0.35">
       <c r="B9" s="6"/>
       <c r="C9" s="10"/>
-      <c r="D9" s="24"/>
+      <c r="D9" s="10"/>
       <c r="E9" s="6"/>
       <c r="F9" s="10"/>
-      <c r="G9" s="24"/>
+      <c r="G9" s="10"/>
       <c r="H9" s="6"/>
       <c r="I9" s="10"/>
-      <c r="J9" s="24"/>
+      <c r="J9" s="10"/>
       <c r="K9" s="6"/>
       <c r="L9" s="10"/>
-      <c r="M9" s="24"/>
+      <c r="M9" s="10"/>
       <c r="N9" s="6"/>
       <c r="O9" s="10"/>
-      <c r="P9" s="24"/>
+      <c r="P9" s="10"/>
       <c r="Q9" s="6"/>
       <c r="R9" s="10"/>
-      <c r="S9" s="24"/>
+      <c r="S9" s="10"/>
       <c r="T9" s="6"/>
       <c r="U9" s="10"/>
-      <c r="V9" s="24"/>
+      <c r="V9" s="10"/>
       <c r="W9" s="6"/>
       <c r="X9" s="10"/>
-      <c r="Y9" s="24"/>
+      <c r="Y9" s="10"/>
       <c r="Z9" s="6"/>
       <c r="AA9" s="10"/>
-      <c r="AB9" s="24"/>
+      <c r="AB9" s="10"/>
       <c r="AC9" s="6"/>
       <c r="AD9" s="10"/>
-      <c r="AE9" s="24"/>
-    </row>
-    <row r="10" spans="1:31" x14ac:dyDescent="0.35">
-      <c r="A10" s="1" t="s">
+      <c r="AE9" s="10"/>
+      <c r="AF9" s="39"/>
+    </row>
+    <row r="10" spans="1:32" x14ac:dyDescent="0.35">
+      <c r="A10" s="16" t="s">
+        <v>41</v>
+      </c>
+      <c r="B10" s="16"/>
+      <c r="C10" s="17"/>
+      <c r="D10" s="34"/>
+      <c r="E10" s="16"/>
+      <c r="F10" s="17"/>
+      <c r="G10" s="34"/>
+      <c r="H10" s="16"/>
+      <c r="I10" s="17"/>
+      <c r="J10" s="34"/>
+      <c r="K10" s="16"/>
+      <c r="L10" s="17"/>
+      <c r="M10" s="34"/>
+      <c r="N10" s="16"/>
+      <c r="O10" s="17"/>
+      <c r="P10" s="34"/>
+      <c r="Q10" s="16"/>
+      <c r="R10" s="17"/>
+      <c r="S10" s="34"/>
+      <c r="T10" s="16"/>
+      <c r="U10" s="17"/>
+      <c r="V10" s="34"/>
+      <c r="W10" s="16"/>
+      <c r="X10" s="17"/>
+      <c r="Y10" s="34"/>
+      <c r="Z10" s="16"/>
+      <c r="AA10" s="17"/>
+      <c r="AB10" s="34"/>
+      <c r="AC10" s="16"/>
+      <c r="AD10" s="17"/>
+      <c r="AE10" s="34"/>
+      <c r="AF10" s="39"/>
+    </row>
+    <row r="11" spans="1:32" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A11" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="B11" s="6">
+        <v>0.4</v>
+      </c>
+      <c r="C11" s="10">
+        <v>0.15730337078651599</v>
+      </c>
+      <c r="D11" s="10">
+        <v>0.65116279069767402</v>
+      </c>
+      <c r="E11" s="6">
+        <v>0.40845070422535201</v>
+      </c>
+      <c r="F11" s="10">
+        <v>0.16571428571428501</v>
+      </c>
+      <c r="G11" s="10">
+        <v>0.64444444444444404</v>
+      </c>
+      <c r="H11" s="6">
+        <v>0.42349726775956198</v>
+      </c>
+      <c r="I11" s="10">
+        <v>0.16666666666666599</v>
+      </c>
+      <c r="J11" s="10">
+        <v>0.688888888888888</v>
+      </c>
+      <c r="K11" s="6">
+        <v>0.44789762340036499</v>
+      </c>
+      <c r="L11" s="10">
+        <v>0.15960912052117199</v>
+      </c>
+      <c r="M11" s="10">
+        <v>0.81666666666666599</v>
+      </c>
+      <c r="N11" s="6">
+        <v>0.44811320754716899</v>
+      </c>
+      <c r="O11" s="10">
+        <v>0.161016949152542</v>
+      </c>
+      <c r="P11" s="10">
+        <v>0.80851063829787195</v>
+      </c>
+      <c r="Q11" s="6">
+        <v>0.40935672514619798</v>
+      </c>
+      <c r="R11" s="10">
+        <v>0.160919540229885</v>
+      </c>
+      <c r="S11" s="10">
+        <v>0.66666666666666596</v>
+      </c>
+      <c r="T11" s="6">
+        <v>0.42525773195876199</v>
+      </c>
+      <c r="U11" s="10">
+        <v>0.16176470588235201</v>
+      </c>
+      <c r="V11" s="10">
+        <v>0.71739130434782505</v>
+      </c>
+      <c r="W11" s="6">
+        <v>0.35175879396984899</v>
+      </c>
+      <c r="X11" s="10">
+        <v>0.123893805309734</v>
+      </c>
+      <c r="Y11" s="10">
+        <v>0.65116279069767402</v>
+      </c>
+      <c r="Z11" s="6">
+        <v>0.40816326530612201</v>
+      </c>
+      <c r="AA11" s="10">
+        <v>0.15686274509803899</v>
+      </c>
+      <c r="AB11" s="10">
+        <v>0.680851063829787</v>
+      </c>
+      <c r="AC11" s="6">
+        <v>0.37804878048780399</v>
+      </c>
+      <c r="AD11" s="10">
+        <v>0.13963963963963899</v>
+      </c>
+      <c r="AE11" s="10">
+        <v>0.659574468085106</v>
+      </c>
+      <c r="AF11" s="3"/>
+    </row>
+    <row r="12" spans="1:32" x14ac:dyDescent="0.35">
+      <c r="A12" s="3"/>
+      <c r="B12" s="6"/>
+      <c r="C12" s="10"/>
+      <c r="D12" s="22"/>
+      <c r="E12" s="6"/>
+      <c r="F12" s="10"/>
+      <c r="G12" s="22"/>
+      <c r="H12" s="6"/>
+      <c r="I12" s="10"/>
+      <c r="J12" s="22"/>
+      <c r="K12" s="6"/>
+      <c r="L12" s="10"/>
+      <c r="M12" s="22"/>
+      <c r="N12" s="6"/>
+      <c r="O12" s="10"/>
+      <c r="P12" s="22"/>
+      <c r="Q12" s="6"/>
+      <c r="R12" s="10"/>
+      <c r="S12" s="22"/>
+      <c r="T12" s="6"/>
+      <c r="U12" s="10"/>
+      <c r="V12" s="22"/>
+      <c r="W12" s="6"/>
+      <c r="X12" s="10"/>
+      <c r="Y12" s="22"/>
+      <c r="Z12" s="6"/>
+      <c r="AA12" s="10"/>
+      <c r="AB12" s="22"/>
+      <c r="AC12" s="6"/>
+      <c r="AD12" s="10"/>
+      <c r="AE12" s="22"/>
+      <c r="AF12" s="39"/>
+    </row>
+    <row r="13" spans="1:32" x14ac:dyDescent="0.35">
+      <c r="A13" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="B10" s="1"/>
-      <c r="C10" s="9"/>
-      <c r="D10" s="2"/>
-      <c r="E10" s="1"/>
-      <c r="F10" s="9"/>
-      <c r="G10" s="2"/>
-      <c r="H10" s="1"/>
-      <c r="I10" s="9"/>
-      <c r="J10" s="2"/>
-      <c r="K10" s="1"/>
-      <c r="L10" s="9"/>
-      <c r="M10" s="2"/>
-      <c r="N10" s="1"/>
-      <c r="O10" s="9"/>
-      <c r="P10" s="2"/>
-      <c r="Q10" s="1"/>
-      <c r="R10" s="9"/>
-      <c r="S10" s="2"/>
-      <c r="T10" s="1"/>
-      <c r="U10" s="9"/>
-      <c r="V10" s="2"/>
-      <c r="W10" s="1"/>
-      <c r="X10" s="9"/>
-      <c r="Y10" s="2"/>
-      <c r="Z10" s="1"/>
-      <c r="AA10" s="9"/>
-      <c r="AB10" s="2"/>
-      <c r="AC10" s="1"/>
-      <c r="AD10" s="9"/>
-      <c r="AE10" s="2"/>
-    </row>
-    <row r="11" spans="1:31" x14ac:dyDescent="0.35">
-      <c r="A11" s="3" t="s">
+      <c r="B13" s="1"/>
+      <c r="C13" s="9"/>
+      <c r="D13" s="2"/>
+      <c r="E13" s="1"/>
+      <c r="F13" s="9"/>
+      <c r="G13" s="2"/>
+      <c r="H13" s="1"/>
+      <c r="I13" s="9"/>
+      <c r="J13" s="2"/>
+      <c r="K13" s="1"/>
+      <c r="L13" s="9"/>
+      <c r="M13" s="2"/>
+      <c r="N13" s="1"/>
+      <c r="O13" s="9"/>
+      <c r="P13" s="2"/>
+      <c r="Q13" s="1"/>
+      <c r="R13" s="9"/>
+      <c r="S13" s="2"/>
+      <c r="T13" s="1"/>
+      <c r="U13" s="9"/>
+      <c r="V13" s="2"/>
+      <c r="W13" s="1"/>
+      <c r="X13" s="9"/>
+      <c r="Y13" s="2"/>
+      <c r="Z13" s="1"/>
+      <c r="AA13" s="9"/>
+      <c r="AB13" s="2"/>
+      <c r="AC13" s="1"/>
+      <c r="AD13" s="9"/>
+      <c r="AE13" s="2"/>
+      <c r="AF13" s="39"/>
+    </row>
+    <row r="14" spans="1:32" x14ac:dyDescent="0.35">
+      <c r="A14" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="B11" s="3">
+      <c r="B14" s="6">
         <v>0.35971223021582699</v>
       </c>
-      <c r="C11" s="5">
+      <c r="C14" s="10">
         <v>0.140845070422535</v>
       </c>
-      <c r="D11" s="32">
+      <c r="D14" s="22">
         <v>0.58823529411764697</v>
       </c>
-      <c r="E11" s="3">
+      <c r="E14" s="6">
         <v>0.40404040404040398</v>
       </c>
-      <c r="F11" s="5">
+      <c r="F14" s="10">
         <v>0.16551724137931001</v>
       </c>
-      <c r="G11" s="32">
+      <c r="G14" s="22">
         <v>0.63157894736842102</v>
       </c>
-      <c r="H11" s="3">
+      <c r="H14" s="6">
         <v>0.41800643086816702</v>
       </c>
-      <c r="I11" s="5">
+      <c r="I14" s="10">
         <v>0.17218543046357601</v>
       </c>
-      <c r="J11" s="32">
+      <c r="J14" s="22">
         <v>0.65</v>
       </c>
-      <c r="K11" s="3">
+      <c r="K14" s="6">
         <v>0.46875</v>
       </c>
-      <c r="L11" s="5">
+      <c r="L14" s="10">
         <v>0.164383561643835</v>
       </c>
-      <c r="M11" s="32">
+      <c r="M14" s="22">
         <v>0.87272727272727202</v>
       </c>
-      <c r="N11" s="3">
+      <c r="N14" s="6">
         <v>0.323033707865168</v>
       </c>
-      <c r="O11" s="5">
+      <c r="O14" s="10">
         <v>0.106481481481481</v>
       </c>
-      <c r="P11" s="32">
+      <c r="P14" s="22">
         <v>0.65714285714285703</v>
       </c>
-      <c r="Q11" s="3">
+      <c r="Q14" s="6">
         <v>0.396039603960396</v>
       </c>
-      <c r="R11" s="5">
+      <c r="R14" s="10">
         <v>0.15094339622641501</v>
       </c>
-      <c r="S11" s="32">
+      <c r="S14" s="22">
         <v>0.66666666666666596</v>
       </c>
-      <c r="T11" s="3">
+      <c r="T14" s="6">
         <v>0.46218487394957902</v>
       </c>
-      <c r="U11" s="5">
+      <c r="U14" s="10">
         <v>0.178378378378378</v>
       </c>
-      <c r="V11" s="32">
+      <c r="V14" s="22">
         <v>0.76744186046511598</v>
       </c>
-      <c r="W11" s="3">
+      <c r="W14" s="6">
         <v>0.352112676056337</v>
       </c>
-      <c r="X11" s="5">
+      <c r="X14" s="10">
         <v>0.12562814070351699</v>
       </c>
-      <c r="Y11" s="32">
+      <c r="Y14" s="22">
         <v>0.64102564102564097</v>
       </c>
-      <c r="Z11" s="3">
+      <c r="Z14" s="6">
         <v>0.38834951456310601</v>
       </c>
-      <c r="AA11" s="5">
+      <c r="AA14" s="10">
         <v>0.152866242038216</v>
       </c>
-      <c r="AB11" s="32">
+      <c r="AB14" s="22">
         <v>0.63157894736842102</v>
       </c>
-      <c r="AC11" s="3">
+      <c r="AC14" s="6">
         <v>0.44757033248081801</v>
       </c>
-      <c r="AD11" s="5">
+      <c r="AD14" s="10">
         <v>0.16587677725118399</v>
       </c>
-      <c r="AE11" s="32">
+      <c r="AE14" s="22">
         <v>0.77777777777777701</v>
       </c>
-    </row>
-    <row r="12" spans="1:31" x14ac:dyDescent="0.35">
-      <c r="A12" s="3"/>
-      <c r="B12" s="3"/>
-      <c r="D12" s="32"/>
-      <c r="E12" s="3"/>
-      <c r="G12" s="32"/>
-      <c r="H12" s="3"/>
-      <c r="J12" s="32"/>
-      <c r="K12" s="3"/>
-      <c r="M12" s="32"/>
-      <c r="N12" s="3"/>
-      <c r="P12" s="32"/>
-      <c r="Q12" s="3"/>
-      <c r="S12" s="32"/>
-      <c r="T12" s="3"/>
-      <c r="V12" s="32"/>
-      <c r="W12" s="3"/>
-      <c r="Y12" s="32"/>
-      <c r="Z12" s="3"/>
-      <c r="AB12" s="32"/>
-      <c r="AC12" s="3"/>
-      <c r="AE12" s="32"/>
-    </row>
-    <row r="13" spans="1:31" x14ac:dyDescent="0.35">
-      <c r="A13" s="1" t="s">
+      <c r="AF14" s="39"/>
+    </row>
+    <row r="15" spans="1:32" x14ac:dyDescent="0.35">
+      <c r="A15" s="3"/>
+      <c r="B15" s="3"/>
+      <c r="D15" s="28"/>
+      <c r="E15" s="3"/>
+      <c r="G15" s="28"/>
+      <c r="H15" s="3"/>
+      <c r="J15" s="28"/>
+      <c r="K15" s="3"/>
+      <c r="M15" s="28"/>
+      <c r="N15" s="3"/>
+      <c r="P15" s="28"/>
+      <c r="Q15" s="3"/>
+      <c r="S15" s="28"/>
+      <c r="T15" s="3"/>
+      <c r="V15" s="28"/>
+      <c r="W15" s="3"/>
+      <c r="Y15" s="28"/>
+      <c r="Z15" s="3"/>
+      <c r="AB15" s="28"/>
+      <c r="AC15" s="3"/>
+      <c r="AE15" s="28"/>
+      <c r="AF15" s="39"/>
+    </row>
+    <row r="16" spans="1:32" x14ac:dyDescent="0.35">
+      <c r="A16" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="B13" s="7"/>
-      <c r="C13" s="11"/>
-      <c r="D13" s="8"/>
-      <c r="E13" s="7"/>
-      <c r="F13" s="11"/>
-      <c r="G13" s="8"/>
-      <c r="H13" s="7"/>
-      <c r="I13" s="11"/>
-      <c r="J13" s="8"/>
-      <c r="K13" s="7"/>
-      <c r="L13" s="11"/>
-      <c r="M13" s="8"/>
-      <c r="N13" s="7"/>
-      <c r="O13" s="11"/>
-      <c r="P13" s="8"/>
-      <c r="Q13" s="7"/>
-      <c r="R13" s="11"/>
-      <c r="S13" s="8"/>
-      <c r="T13" s="7"/>
-      <c r="U13" s="11"/>
-      <c r="V13" s="8"/>
-      <c r="W13" s="7"/>
-      <c r="X13" s="11"/>
-      <c r="Y13" s="8"/>
-      <c r="Z13" s="7"/>
-      <c r="AA13" s="11"/>
-      <c r="AB13" s="8"/>
-      <c r="AC13" s="7"/>
-      <c r="AD13" s="11"/>
-      <c r="AE13" s="8"/>
-    </row>
-    <row r="14" spans="1:31" x14ac:dyDescent="0.35">
-      <c r="A14" s="16" t="s">
+      <c r="B16" s="7"/>
+      <c r="C16" s="11"/>
+      <c r="D16" s="8"/>
+      <c r="E16" s="7"/>
+      <c r="F16" s="11"/>
+      <c r="G16" s="8"/>
+      <c r="H16" s="7"/>
+      <c r="I16" s="11"/>
+      <c r="J16" s="8"/>
+      <c r="K16" s="7"/>
+      <c r="L16" s="11"/>
+      <c r="M16" s="8"/>
+      <c r="N16" s="7"/>
+      <c r="O16" s="11"/>
+      <c r="P16" s="8"/>
+      <c r="Q16" s="7"/>
+      <c r="R16" s="11"/>
+      <c r="S16" s="8"/>
+      <c r="T16" s="7"/>
+      <c r="U16" s="11"/>
+      <c r="V16" s="8"/>
+      <c r="W16" s="7"/>
+      <c r="X16" s="11"/>
+      <c r="Y16" s="8"/>
+      <c r="Z16" s="7"/>
+      <c r="AA16" s="11"/>
+      <c r="AB16" s="8"/>
+      <c r="AC16" s="7"/>
+      <c r="AD16" s="11"/>
+      <c r="AE16" s="8"/>
+      <c r="AF16" s="39"/>
+    </row>
+    <row r="17" spans="1:32" x14ac:dyDescent="0.35">
+      <c r="A17" s="15" t="s">
         <v>23</v>
       </c>
-      <c r="B14" s="16">
+      <c r="B17" s="13">
         <v>0.47560975609756101</v>
       </c>
-      <c r="C14" s="22">
+      <c r="C17" s="14">
         <v>0.185714285714285</v>
       </c>
-      <c r="D14" s="33">
+      <c r="D17" s="21">
         <v>0.78</v>
       </c>
-      <c r="E14" s="16">
+      <c r="E17" s="13">
         <v>0.49757281553397997</v>
       </c>
-      <c r="F14" s="22">
+      <c r="F17" s="14">
         <v>0.19339622641509399</v>
       </c>
-      <c r="G14" s="33">
+      <c r="G17" s="21">
         <v>0.82</v>
       </c>
-      <c r="H14" s="16">
+      <c r="H17" s="13">
         <v>0.51094890510948898</v>
       </c>
-      <c r="I14" s="22">
+      <c r="I17" s="14">
         <v>0.199052132701421</v>
       </c>
-      <c r="J14" s="33">
+      <c r="J17" s="21">
         <v>0.84</v>
       </c>
-      <c r="K14" s="16">
+      <c r="K17" s="13">
         <v>0.47706422018348599</v>
       </c>
-      <c r="L14" s="22">
+      <c r="L17" s="14">
         <v>0.168284789644012</v>
       </c>
-      <c r="M14" s="33">
+      <c r="M17" s="21">
         <v>0.88135593220338904</v>
       </c>
-      <c r="N14" s="16">
+      <c r="N17" s="13">
         <v>0.418454935622317</v>
       </c>
-      <c r="O14" s="22">
+      <c r="O17" s="14">
         <v>0.14233576642335699</v>
       </c>
-      <c r="P14" s="33">
+      <c r="P17" s="21">
         <v>0.8125</v>
       </c>
-      <c r="Q14" s="16">
+      <c r="Q17" s="13">
         <v>0.42857142857142799</v>
       </c>
-      <c r="R14" s="22">
+      <c r="R17" s="14">
         <v>0.15207373271889399</v>
       </c>
-      <c r="S14" s="33">
+      <c r="S17" s="21">
         <v>0.78571428571428503</v>
       </c>
-      <c r="T14" s="16">
+      <c r="T17" s="13">
         <v>0.53738317757009302</v>
       </c>
-      <c r="U14" s="22">
+      <c r="U17" s="14">
         <v>0.20535714285714199</v>
       </c>
-      <c r="V14" s="33">
+      <c r="V17" s="21">
         <v>0.90196078431372495</v>
       </c>
-      <c r="W14" s="16">
+      <c r="W17" s="13">
         <v>0.51229508196721296</v>
       </c>
-      <c r="X14" s="22">
+      <c r="X17" s="14">
         <v>0.19841269841269801</v>
       </c>
-      <c r="Y14" s="33">
+      <c r="Y17" s="21">
         <v>0.84745762711864303</v>
       </c>
-      <c r="Z14" s="16">
+      <c r="Z17" s="13">
         <v>0.49118387909319899</v>
       </c>
-      <c r="AA14" s="22">
+      <c r="AA17" s="14">
         <v>0.194029850746268</v>
       </c>
-      <c r="AB14" s="33">
+      <c r="AB17" s="21">
         <v>0.79591836734693799</v>
       </c>
-      <c r="AC14" s="16">
+      <c r="AC17" s="13">
         <v>0.48625792811839302</v>
       </c>
-      <c r="AD14" s="22">
+      <c r="AD17" s="14">
         <v>0.176245210727969</v>
       </c>
-      <c r="AE14" s="33">
+      <c r="AE17" s="21">
         <v>0.86792452830188604</v>
       </c>
-    </row>
-    <row r="15" spans="1:31" x14ac:dyDescent="0.35">
-      <c r="A15" s="25" t="s">
+      <c r="AF17" s="39"/>
+    </row>
+    <row r="18" spans="1:32" x14ac:dyDescent="0.35">
+      <c r="A18" s="23" t="s">
         <v>24</v>
       </c>
-      <c r="B15" s="25">
+      <c r="B18" s="24">
         <v>0.29255319148936099</v>
       </c>
-      <c r="C15" s="26">
+      <c r="C18" s="25">
         <v>0.16176470588235201</v>
       </c>
-      <c r="D15" s="38">
+      <c r="D18" s="26">
         <v>0.36666666666666597</v>
       </c>
-      <c r="E15" s="25">
+      <c r="E18" s="24">
         <v>0.25280898876404401</v>
       </c>
-      <c r="F15" s="26">
+      <c r="F18" s="25">
         <v>0.13636363636363599</v>
       </c>
-      <c r="G15" s="38">
+      <c r="G18" s="26">
         <v>0.32142857142857101</v>
       </c>
-      <c r="H15" s="25">
+      <c r="H18" s="24">
         <v>0.39408866995073799</v>
       </c>
-      <c r="I15" s="26">
+      <c r="I18" s="25">
         <v>0.22535211267605601</v>
       </c>
-      <c r="J15" s="38">
+      <c r="J18" s="26">
         <v>0.48484848484848397</v>
       </c>
-      <c r="K15" s="25">
+      <c r="K18" s="24">
         <v>0.39432176656151402</v>
       </c>
-      <c r="L15" s="26">
+      <c r="L18" s="25">
         <v>0.15151515151515099</v>
       </c>
-      <c r="M15" s="38">
+      <c r="M18" s="26">
         <v>0.65789473684210498</v>
       </c>
-      <c r="N15" s="25">
+      <c r="N18" s="24">
         <v>0.36170212765957399</v>
       </c>
-      <c r="O15" s="26">
+      <c r="O18" s="25">
         <v>0.153153153153153</v>
       </c>
-      <c r="P15" s="38">
+      <c r="P18" s="26">
         <v>0.54838709677419295</v>
       </c>
-      <c r="Q15" s="25">
+      <c r="Q18" s="24">
         <v>0.34574468085106302</v>
       </c>
-      <c r="R15" s="26">
+      <c r="R18" s="25">
         <v>0.180555555555555</v>
       </c>
-      <c r="S15" s="38">
+      <c r="S18" s="26">
         <v>0.44827586206896503</v>
       </c>
-      <c r="T15" s="25">
+      <c r="T18" s="24">
         <v>0.34403669724770602</v>
       </c>
-      <c r="U15" s="26">
+      <c r="U18" s="25">
         <v>0.159574468085106</v>
       </c>
-      <c r="V15" s="38">
+      <c r="V18" s="26">
         <v>0.483870967741935</v>
       </c>
-      <c r="W15" s="25">
+      <c r="W18" s="24">
         <v>0.30232558139534799</v>
       </c>
-      <c r="X15" s="26">
+      <c r="X18" s="25">
         <v>0.14285714285714199</v>
       </c>
-      <c r="Y15" s="38">
+      <c r="Y18" s="26">
         <v>0.41935483870967699</v>
       </c>
-      <c r="Z15" s="25">
+      <c r="Z18" s="24">
         <v>0.28985507246376802</v>
       </c>
-      <c r="AA15" s="26">
+      <c r="AA18" s="25">
         <v>0.13793103448275801</v>
       </c>
-      <c r="AB15" s="38">
+      <c r="AB18" s="26">
         <v>0.4</v>
       </c>
-      <c r="AC15" s="25">
+      <c r="AC18" s="24">
         <v>0.28985507246376802</v>
       </c>
-      <c r="AD15" s="26">
+      <c r="AD18" s="25">
         <v>0.13186813186813101</v>
       </c>
-      <c r="AE15" s="38">
+      <c r="AE18" s="26">
         <v>0.41379310344827502</v>
       </c>
-    </row>
-    <row r="16" spans="1:31" x14ac:dyDescent="0.35">
-      <c r="A16"/>
-      <c r="B16"/>
-      <c r="C16"/>
-      <c r="D16"/>
-      <c r="E16"/>
-      <c r="F16"/>
-      <c r="G16"/>
-      <c r="H16"/>
-      <c r="I16"/>
-      <c r="J16"/>
-      <c r="K16"/>
-      <c r="L16"/>
-      <c r="M16"/>
-      <c r="N16"/>
-      <c r="O16"/>
-      <c r="P16"/>
-      <c r="Q16"/>
-      <c r="R16"/>
-      <c r="S16"/>
-      <c r="T16"/>
-      <c r="U16"/>
-      <c r="V16"/>
-      <c r="W16"/>
-      <c r="X16"/>
-      <c r="Y16"/>
-      <c r="Z16"/>
-      <c r="AA16"/>
-      <c r="AB16"/>
-      <c r="AC16"/>
-      <c r="AD16"/>
-      <c r="AE16"/>
-    </row>
-    <row r="17" spans="1:31" x14ac:dyDescent="0.35">
-      <c r="A17" s="13"/>
-      <c r="B17" s="13"/>
-      <c r="C17" s="13"/>
-      <c r="D17" s="13"/>
-      <c r="E17" s="13"/>
-      <c r="F17" s="13"/>
-      <c r="G17" s="13"/>
-      <c r="H17" s="13"/>
-      <c r="I17" s="13"/>
-      <c r="J17" s="13"/>
-      <c r="K17" s="13"/>
-      <c r="L17" s="13"/>
-      <c r="M17" s="13"/>
-      <c r="N17" s="13"/>
-      <c r="O17" s="13"/>
-      <c r="P17" s="13"/>
-      <c r="Q17" s="13"/>
-      <c r="R17" s="13"/>
-      <c r="S17" s="13"/>
-      <c r="T17" s="13"/>
-      <c r="U17" s="13"/>
-      <c r="V17" s="13"/>
-      <c r="W17" s="13"/>
-      <c r="X17" s="13"/>
-      <c r="Y17" s="13"/>
-      <c r="Z17" s="13"/>
-      <c r="AA17" s="13"/>
-      <c r="AB17" s="13"/>
-      <c r="AC17" s="13"/>
-      <c r="AD17" s="13"/>
-      <c r="AE17" s="13"/>
-    </row>
-    <row r="18" spans="1:31" x14ac:dyDescent="0.35">
-      <c r="A18" s="30"/>
-      <c r="B18" s="30"/>
-      <c r="C18" s="30"/>
-      <c r="D18" s="30"/>
-      <c r="E18" s="30"/>
-      <c r="F18" s="30"/>
-      <c r="G18" s="30"/>
-      <c r="H18" s="30"/>
-      <c r="I18" s="30"/>
-      <c r="J18" s="30"/>
-      <c r="K18" s="30"/>
-      <c r="L18" s="30"/>
-      <c r="M18" s="30"/>
-      <c r="N18" s="30"/>
-      <c r="O18" s="30"/>
-      <c r="P18" s="30"/>
-      <c r="Q18" s="30"/>
-      <c r="R18" s="30"/>
-      <c r="S18" s="30"/>
-      <c r="T18" s="30"/>
-      <c r="U18" s="30"/>
-      <c r="V18" s="30"/>
-      <c r="W18" s="30"/>
-      <c r="X18" s="30"/>
-      <c r="Y18" s="30"/>
-      <c r="Z18" s="30"/>
-      <c r="AA18" s="30"/>
-      <c r="AB18" s="30"/>
-      <c r="AC18" s="30"/>
-      <c r="AD18" s="30"/>
-      <c r="AE18" s="30"/>
-    </row>
-    <row r="19" spans="1:31" ht="21" x14ac:dyDescent="0.5">
-      <c r="A19" s="35" t="s">
+      <c r="AF18" s="39"/>
+    </row>
+    <row r="19" spans="1:32" x14ac:dyDescent="0.35">
+      <c r="A19"/>
+      <c r="B19"/>
+      <c r="C19"/>
+      <c r="D19"/>
+      <c r="E19"/>
+      <c r="F19"/>
+      <c r="G19"/>
+      <c r="H19"/>
+      <c r="I19"/>
+      <c r="J19"/>
+      <c r="K19"/>
+      <c r="L19"/>
+      <c r="M19"/>
+      <c r="N19"/>
+      <c r="O19"/>
+      <c r="P19"/>
+      <c r="Q19"/>
+      <c r="R19"/>
+      <c r="S19"/>
+      <c r="T19"/>
+      <c r="U19"/>
+      <c r="V19"/>
+      <c r="W19"/>
+      <c r="X19"/>
+      <c r="Y19"/>
+      <c r="Z19"/>
+      <c r="AA19"/>
+      <c r="AB19"/>
+      <c r="AC19"/>
+      <c r="AD19"/>
+      <c r="AE19"/>
+    </row>
+    <row r="20" spans="1:32" x14ac:dyDescent="0.35">
+      <c r="A20" s="12"/>
+      <c r="B20" s="12"/>
+      <c r="C20" s="12"/>
+      <c r="D20" s="12"/>
+      <c r="E20" s="12"/>
+      <c r="F20" s="12"/>
+      <c r="G20" s="12"/>
+      <c r="H20" s="12"/>
+      <c r="I20" s="12"/>
+      <c r="J20" s="12"/>
+      <c r="K20" s="12"/>
+      <c r="L20" s="12"/>
+      <c r="M20" s="12"/>
+      <c r="N20" s="12"/>
+      <c r="O20" s="12"/>
+      <c r="P20" s="12"/>
+      <c r="Q20" s="12"/>
+      <c r="R20" s="12"/>
+      <c r="S20" s="12"/>
+      <c r="T20" s="12"/>
+      <c r="U20" s="12"/>
+      <c r="V20" s="12"/>
+      <c r="W20" s="12"/>
+      <c r="X20" s="12"/>
+      <c r="Y20" s="12"/>
+      <c r="Z20" s="12"/>
+      <c r="AA20" s="12"/>
+      <c r="AB20" s="12"/>
+      <c r="AC20" s="12"/>
+      <c r="AD20" s="12"/>
+      <c r="AE20" s="12"/>
+    </row>
+    <row r="21" spans="1:32" x14ac:dyDescent="0.35">
+      <c r="A21" s="27"/>
+      <c r="B21" s="27"/>
+      <c r="C21" s="27"/>
+      <c r="D21" s="27"/>
+      <c r="E21" s="27"/>
+      <c r="F21" s="27"/>
+      <c r="G21" s="27"/>
+      <c r="H21" s="27"/>
+      <c r="I21" s="27"/>
+      <c r="J21" s="27"/>
+      <c r="K21" s="27"/>
+      <c r="L21" s="27"/>
+      <c r="M21" s="27"/>
+      <c r="N21" s="27"/>
+      <c r="O21" s="27"/>
+      <c r="P21" s="27"/>
+      <c r="Q21" s="27"/>
+      <c r="R21" s="27"/>
+      <c r="S21" s="27"/>
+      <c r="T21" s="27"/>
+      <c r="U21" s="27"/>
+      <c r="V21" s="27"/>
+      <c r="W21" s="27"/>
+      <c r="X21" s="27"/>
+      <c r="Y21" s="27"/>
+      <c r="Z21" s="27"/>
+      <c r="AA21" s="27"/>
+      <c r="AB21" s="27"/>
+      <c r="AC21" s="27"/>
+      <c r="AD21" s="27"/>
+      <c r="AE21" s="27"/>
+    </row>
+    <row r="22" spans="1:32" ht="21" x14ac:dyDescent="0.5">
+      <c r="A22" s="29" t="s">
         <v>39</v>
       </c>
-      <c r="B19" s="39"/>
-      <c r="C19" s="39"/>
-      <c r="D19" s="39"/>
-      <c r="E19" s="39"/>
-      <c r="F19" s="39"/>
-      <c r="G19" s="39"/>
-      <c r="H19" s="39"/>
-      <c r="I19" s="39"/>
-      <c r="J19" s="39"/>
-      <c r="K19" s="39"/>
-      <c r="L19" s="39"/>
-      <c r="M19" s="39"/>
-      <c r="N19" s="39"/>
-      <c r="O19" s="39"/>
-      <c r="P19" s="39"/>
-      <c r="Q19" s="39"/>
-      <c r="R19" s="39"/>
-      <c r="S19" s="39"/>
-      <c r="T19" s="39"/>
-      <c r="U19" s="39"/>
-      <c r="V19" s="39"/>
-      <c r="W19" s="39"/>
-      <c r="X19" s="39"/>
-      <c r="Y19" s="39"/>
-      <c r="Z19" s="39"/>
-      <c r="AA19" s="39"/>
-      <c r="AB19" s="39"/>
-      <c r="AC19" s="39"/>
-      <c r="AD19" s="39"/>
-      <c r="AE19" s="40"/>
-    </row>
-    <row r="20" spans="1:31" x14ac:dyDescent="0.35">
-      <c r="A20" s="3"/>
-      <c r="B20" s="34" t="s">
+      <c r="B22" s="32"/>
+      <c r="C22" s="32"/>
+      <c r="D22" s="32"/>
+      <c r="E22" s="32"/>
+      <c r="F22" s="32"/>
+      <c r="G22" s="32"/>
+      <c r="H22" s="32"/>
+      <c r="I22" s="32"/>
+      <c r="J22" s="32"/>
+      <c r="K22" s="32"/>
+      <c r="L22" s="32"/>
+      <c r="M22" s="32"/>
+      <c r="N22" s="32"/>
+      <c r="O22" s="32"/>
+      <c r="P22" s="32"/>
+      <c r="Q22" s="32"/>
+      <c r="R22" s="32"/>
+      <c r="S22" s="32"/>
+      <c r="T22" s="32"/>
+      <c r="U22" s="32"/>
+      <c r="V22" s="32"/>
+      <c r="W22" s="32"/>
+      <c r="X22" s="32"/>
+      <c r="Y22" s="32"/>
+      <c r="Z22" s="32"/>
+      <c r="AA22" s="32"/>
+      <c r="AB22" s="32"/>
+      <c r="AC22" s="32"/>
+      <c r="AD22" s="32"/>
+      <c r="AE22" s="33"/>
+    </row>
+    <row r="23" spans="1:32" x14ac:dyDescent="0.35">
+      <c r="A23" s="3"/>
+      <c r="B23" s="36" t="s">
         <v>0</v>
       </c>
-      <c r="C20" s="12"/>
-      <c r="D20" s="31"/>
-      <c r="E20" s="34" t="s">
+      <c r="C23" s="37"/>
+      <c r="D23" s="38"/>
+      <c r="E23" s="36" t="s">
         <v>4</v>
       </c>
-      <c r="F20" s="12"/>
-      <c r="G20" s="31"/>
-      <c r="H20" s="34" t="s">
+      <c r="F23" s="37"/>
+      <c r="G23" s="38"/>
+      <c r="H23" s="36" t="s">
         <v>5</v>
       </c>
-      <c r="I20" s="12"/>
-      <c r="J20" s="31"/>
-      <c r="K20" s="34" t="s">
+      <c r="I23" s="37"/>
+      <c r="J23" s="38"/>
+      <c r="K23" s="36" t="s">
         <v>6</v>
       </c>
-      <c r="L20" s="12"/>
-      <c r="M20" s="31"/>
-      <c r="N20" s="34" t="s">
+      <c r="L23" s="37"/>
+      <c r="M23" s="38"/>
+      <c r="N23" s="36" t="s">
         <v>7</v>
       </c>
-      <c r="O20" s="12"/>
-      <c r="P20" s="31"/>
-      <c r="Q20" s="34" t="s">
+      <c r="O23" s="37"/>
+      <c r="P23" s="38"/>
+      <c r="Q23" s="36" t="s">
         <v>8</v>
       </c>
-      <c r="R20" s="12"/>
-      <c r="S20" s="31"/>
-      <c r="T20" s="34" t="s">
+      <c r="R23" s="37"/>
+      <c r="S23" s="38"/>
+      <c r="T23" s="36" t="s">
         <v>9</v>
       </c>
-      <c r="U20" s="12"/>
-      <c r="V20" s="31"/>
-      <c r="W20" s="34" t="s">
+      <c r="U23" s="37"/>
+      <c r="V23" s="38"/>
+      <c r="W23" s="36" t="s">
         <v>10</v>
       </c>
-      <c r="X20" s="12"/>
-      <c r="Y20" s="31"/>
-      <c r="Z20" s="34" t="s">
+      <c r="X23" s="37"/>
+      <c r="Y23" s="38"/>
+      <c r="Z23" s="36" t="s">
         <v>11</v>
       </c>
-      <c r="AA20" s="12"/>
-      <c r="AB20" s="31"/>
-      <c r="AC20" s="34" t="s">
+      <c r="AA23" s="37"/>
+      <c r="AB23" s="38"/>
+      <c r="AC23" s="36" t="s">
         <v>12</v>
       </c>
-      <c r="AD20" s="12"/>
-      <c r="AE20" s="31"/>
-    </row>
-    <row r="21" spans="1:31" x14ac:dyDescent="0.35">
-      <c r="A21" s="3" t="s">
+      <c r="AD23" s="37"/>
+      <c r="AE23" s="38"/>
+    </row>
+    <row r="24" spans="1:32" x14ac:dyDescent="0.35">
+      <c r="A24" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="B21" s="3" t="s">
+      <c r="B24" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="C21" s="5" t="s">
+      <c r="C24" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="D21" s="32" t="s">
+      <c r="D24" s="28" t="s">
         <v>1</v>
       </c>
-      <c r="E21" s="3" t="s">
+      <c r="E24" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="F21" s="5" t="s">
+      <c r="F24" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="G21" s="32" t="s">
+      <c r="G24" s="28" t="s">
         <v>1</v>
       </c>
-      <c r="H21" s="3" t="s">
+      <c r="H24" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="I21" s="5" t="s">
+      <c r="I24" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="J21" s="32" t="s">
+      <c r="J24" s="28" t="s">
         <v>1</v>
       </c>
-      <c r="K21" s="3" t="s">
+      <c r="K24" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="L21" s="5" t="s">
+      <c r="L24" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="M21" s="32" t="s">
+      <c r="M24" s="28" t="s">
         <v>1</v>
       </c>
-      <c r="N21" s="3" t="s">
+      <c r="N24" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="O21" s="5" t="s">
+      <c r="O24" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="P21" s="32" t="s">
+      <c r="P24" s="28" t="s">
         <v>1</v>
       </c>
-      <c r="Q21" s="3" t="s">
+      <c r="Q24" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="R21" s="5" t="s">
+      <c r="R24" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="S21" s="32" t="s">
+      <c r="S24" s="28" t="s">
         <v>1</v>
       </c>
-      <c r="T21" s="3" t="s">
+      <c r="T24" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="U21" s="5" t="s">
+      <c r="U24" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="V21" s="32" t="s">
+      <c r="V24" s="28" t="s">
         <v>1</v>
       </c>
-      <c r="W21" s="3" t="s">
+      <c r="W24" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="X21" s="5" t="s">
+      <c r="X24" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="Y21" s="32" t="s">
+      <c r="Y24" s="28" t="s">
         <v>1</v>
       </c>
-      <c r="Z21" s="3" t="s">
+      <c r="Z24" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="AA21" s="5" t="s">
+      <c r="AA24" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="AB21" s="32" t="s">
+      <c r="AB24" s="28" t="s">
         <v>1</v>
       </c>
-      <c r="AC21" s="3" t="s">
+      <c r="AC24" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="AD21" s="5" t="s">
+      <c r="AD24" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="AE21" s="32" t="s">
+      <c r="AE24" s="28" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:31" x14ac:dyDescent="0.35">
-      <c r="A22" s="17" t="s">
+    <row r="25" spans="1:32" x14ac:dyDescent="0.35">
+      <c r="A25" s="16" t="s">
         <v>17</v>
       </c>
-      <c r="B22" s="19"/>
-      <c r="C22" s="20"/>
-      <c r="D22" s="21"/>
-      <c r="E22" s="19"/>
-      <c r="F22" s="20"/>
-      <c r="G22" s="21"/>
-      <c r="H22" s="19"/>
-      <c r="I22" s="20"/>
-      <c r="J22" s="21"/>
-      <c r="K22" s="19"/>
-      <c r="L22" s="20"/>
-      <c r="M22" s="20"/>
-      <c r="N22" s="19"/>
-      <c r="O22" s="20"/>
-      <c r="P22" s="20"/>
-      <c r="Q22" s="19"/>
-      <c r="R22" s="20"/>
-      <c r="S22" s="20"/>
-      <c r="T22" s="19"/>
-      <c r="U22" s="20"/>
-      <c r="V22" s="20"/>
-      <c r="W22" s="19"/>
-      <c r="X22" s="20"/>
-      <c r="Y22" s="20"/>
-      <c r="Z22" s="19"/>
-      <c r="AA22" s="20"/>
-      <c r="AB22" s="20"/>
-      <c r="AC22" s="19"/>
-      <c r="AD22" s="20"/>
-      <c r="AE22" s="21"/>
-    </row>
-    <row r="23" spans="1:31" x14ac:dyDescent="0.35">
-      <c r="A23" s="16" t="s">
+      <c r="B25" s="18"/>
+      <c r="C25" s="19"/>
+      <c r="D25" s="20"/>
+      <c r="E25" s="18"/>
+      <c r="F25" s="19"/>
+      <c r="G25" s="20"/>
+      <c r="H25" s="18"/>
+      <c r="I25" s="19"/>
+      <c r="J25" s="20"/>
+      <c r="K25" s="18"/>
+      <c r="L25" s="19"/>
+      <c r="M25" s="19"/>
+      <c r="N25" s="18"/>
+      <c r="O25" s="19"/>
+      <c r="P25" s="19"/>
+      <c r="Q25" s="18"/>
+      <c r="R25" s="19"/>
+      <c r="S25" s="19"/>
+      <c r="T25" s="18"/>
+      <c r="U25" s="19"/>
+      <c r="V25" s="19"/>
+      <c r="W25" s="18"/>
+      <c r="X25" s="19"/>
+      <c r="Y25" s="19"/>
+      <c r="Z25" s="18"/>
+      <c r="AA25" s="19"/>
+      <c r="AB25" s="19"/>
+      <c r="AC25" s="18"/>
+      <c r="AD25" s="19"/>
+      <c r="AE25" s="20"/>
+    </row>
+    <row r="26" spans="1:32" x14ac:dyDescent="0.35">
+      <c r="A26" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="B23" s="14">
+      <c r="B26" s="13">
         <v>0.61983471074380103</v>
       </c>
-      <c r="C23" s="15">
+      <c r="C26" s="14">
         <v>0.30612244897959101</v>
       </c>
-      <c r="D23" s="15">
+      <c r="D26" s="14">
         <v>0.83333333333333304</v>
       </c>
-      <c r="E23" s="14">
+      <c r="E26" s="13">
         <v>0.64393939393939303</v>
       </c>
-      <c r="F23" s="15">
+      <c r="F26" s="14">
         <v>0.32692307692307598</v>
       </c>
-      <c r="G23" s="15">
+      <c r="G26" s="14">
         <v>0.85</v>
       </c>
-      <c r="H23" s="14">
+      <c r="H26" s="13">
         <v>0.62992125984251901</v>
       </c>
-      <c r="I23" s="15">
+      <c r="I26" s="14">
         <v>0.31372549019607798</v>
       </c>
-      <c r="J23" s="15">
+      <c r="J26" s="14">
         <v>0.84210526315789402</v>
       </c>
-      <c r="K23" s="14">
+      <c r="K26" s="13">
         <v>0.48275862068965503</v>
       </c>
-      <c r="L23" s="15">
+      <c r="L26" s="14">
         <v>0.19178082191780799</v>
       </c>
-      <c r="M23" s="15">
+      <c r="M26" s="14">
         <v>0.77777777777777701</v>
       </c>
-      <c r="N23" s="14">
+      <c r="N26" s="13">
         <v>0.55555555555555503</v>
       </c>
-      <c r="O23" s="15">
+      <c r="O26" s="14">
         <v>0.25</v>
       </c>
-      <c r="P23" s="15">
+      <c r="P26" s="14">
         <v>0.8</v>
       </c>
-      <c r="Q23" s="14">
+      <c r="Q26" s="13">
         <v>0.64</v>
       </c>
-      <c r="R23" s="15">
+      <c r="R26" s="14">
         <v>0.30188679245283001</v>
       </c>
-      <c r="S23" s="15">
+      <c r="S26" s="14">
         <v>0.88888888888888795</v>
       </c>
-      <c r="T23" s="14">
+      <c r="T26" s="13">
         <v>0.65693430656934304</v>
       </c>
-      <c r="U23" s="15">
+      <c r="U26" s="14">
         <v>0.31578947368421001</v>
       </c>
-      <c r="V23" s="15">
+      <c r="V26" s="14">
         <v>0.9</v>
       </c>
-      <c r="W23" s="14">
+      <c r="W26" s="13">
         <v>0.67307692307692302</v>
       </c>
-      <c r="X23" s="15">
+      <c r="X26" s="14">
         <v>0.328125</v>
       </c>
-      <c r="Y23" s="15">
+      <c r="Y26" s="14">
         <v>0.91304347826086896</v>
       </c>
-      <c r="Z23" s="14">
+      <c r="Z26" s="13">
         <v>0.63432835820895495</v>
       </c>
-      <c r="AA23" s="15">
+      <c r="AA26" s="14">
         <v>0.31481481481481399</v>
       </c>
-      <c r="AB23" s="15">
+      <c r="AB26" s="14">
         <v>0.85</v>
       </c>
-      <c r="AC23" s="14">
+      <c r="AC26" s="13">
         <v>0.55194805194805197</v>
       </c>
-      <c r="AD23" s="15">
+      <c r="AD26" s="14">
         <v>0.24285714285714199</v>
       </c>
-      <c r="AE23" s="23">
+      <c r="AE26" s="21">
         <v>0.80952380952380898</v>
       </c>
     </row>
-    <row r="24" spans="1:31" x14ac:dyDescent="0.35">
-      <c r="A24" s="3" t="s">
+    <row r="27" spans="1:32" x14ac:dyDescent="0.35">
+      <c r="A27" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="B24" s="6">
+      <c r="B27" s="6">
         <v>0.26315789473684198</v>
       </c>
-      <c r="C24" s="10">
+      <c r="C27" s="10">
         <v>0.23076923076923</v>
       </c>
-      <c r="D24" s="10">
+      <c r="D27" s="10">
         <v>0.27272727272727199</v>
       </c>
-      <c r="E24" s="6">
+      <c r="E27" s="6">
         <v>0.32786885245901598</v>
       </c>
-      <c r="F24" s="10">
+      <c r="F27" s="10">
         <v>0.30769230769230699</v>
       </c>
-      <c r="G24" s="10">
+      <c r="G27" s="10">
         <v>0.33333333333333298</v>
       </c>
-      <c r="H24" s="6">
+      <c r="H27" s="6">
         <v>0.24590163934426201</v>
       </c>
-      <c r="I24" s="10">
+      <c r="I27" s="10">
         <v>0.23076923076923</v>
       </c>
-      <c r="J24" s="10">
+      <c r="J27" s="10">
         <v>0.25</v>
       </c>
-      <c r="K24" s="6">
+      <c r="K27" s="6">
         <v>0.38793103448275801</v>
       </c>
-      <c r="L24" s="10">
+      <c r="L27" s="10">
         <v>0.160714285714285</v>
       </c>
-      <c r="M24" s="10">
+      <c r="M27" s="10">
         <v>0.6</v>
       </c>
-      <c r="N24" s="6">
+      <c r="N27" s="6">
         <v>0.38961038961038902</v>
       </c>
-      <c r="O24" s="10">
+      <c r="O27" s="10">
         <v>0.18181818181818099</v>
       </c>
-      <c r="P24" s="10">
+      <c r="P27" s="10">
         <v>0.54545454545454497</v>
       </c>
-      <c r="Q24" s="6">
+      <c r="Q27" s="6">
         <v>0.43103448275862</v>
       </c>
-      <c r="R24" s="10">
+      <c r="R27" s="10">
         <v>0.35714285714285698</v>
       </c>
-      <c r="S24" s="10">
+      <c r="S27" s="10">
         <v>0.45454545454545398</v>
       </c>
-      <c r="T24" s="6">
+      <c r="T27" s="6">
         <v>0.34246575342465702</v>
       </c>
-      <c r="U24" s="10">
+      <c r="U27" s="10">
         <v>0.2</v>
       </c>
-      <c r="V24" s="10">
+      <c r="V27" s="10">
         <v>0.41666666666666602</v>
       </c>
-      <c r="W24" s="6">
+      <c r="W27" s="6">
         <v>0.34482758620689602</v>
       </c>
-      <c r="X24" s="10">
+      <c r="X27" s="10">
         <v>0.22222222222222199</v>
       </c>
-      <c r="Y24" s="10">
+      <c r="Y27" s="10">
         <v>0.4</v>
       </c>
-      <c r="Z24" s="6">
+      <c r="Z27" s="6">
         <v>0.337837837837837</v>
       </c>
-      <c r="AA24" s="10">
+      <c r="AA27" s="10">
         <v>0.19230769230769201</v>
       </c>
-      <c r="AB24" s="10">
+      <c r="AB27" s="10">
         <v>0.41666666666666602</v>
       </c>
-      <c r="AC24" s="6">
+      <c r="AC27" s="6">
         <v>0.36231884057970998</v>
       </c>
-      <c r="AD24" s="10">
+      <c r="AD27" s="10">
         <v>0.2</v>
       </c>
-      <c r="AE24" s="24">
+      <c r="AE27" s="22">
         <v>0.45454545454545398</v>
       </c>
     </row>
-    <row r="25" spans="1:31" x14ac:dyDescent="0.35">
-      <c r="A25" s="3" t="s">
+    <row r="28" spans="1:32" x14ac:dyDescent="0.35">
+      <c r="A28" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="B25" s="6">
+      <c r="B28" s="6">
         <v>0.49180327868852403</v>
       </c>
-      <c r="C25" s="10">
+      <c r="C28" s="10">
         <v>0.46153846153846101</v>
       </c>
-      <c r="D25" s="10">
+      <c r="D28" s="10">
         <v>0.5</v>
       </c>
-      <c r="E25" s="6">
+      <c r="E28" s="6">
         <v>0.3</v>
       </c>
-      <c r="F25" s="10">
+      <c r="F28" s="10">
         <v>0.3</v>
       </c>
-      <c r="G25" s="10">
+      <c r="G28" s="10">
         <v>0.3</v>
       </c>
-      <c r="H25" s="6">
+      <c r="H28" s="6">
         <v>0.40322580645161199</v>
       </c>
-      <c r="I25" s="10">
+      <c r="I28" s="10">
         <v>0.35714285714285698</v>
       </c>
-      <c r="J25" s="10">
+      <c r="J28" s="10">
         <v>0.41666666666666602</v>
       </c>
-      <c r="K25" s="6">
+      <c r="K28" s="6">
         <v>0.51401869158878499</v>
       </c>
-      <c r="L25" s="10">
+      <c r="L28" s="10">
         <v>0.28205128205128199</v>
       </c>
-      <c r="M25" s="10">
+      <c r="M28" s="10">
         <v>0.64705882352941102</v>
       </c>
-      <c r="N25" s="6">
+      <c r="N28" s="6">
         <v>0.42253521126760502</v>
       </c>
-      <c r="O25" s="10">
+      <c r="O28" s="10">
         <v>0.26086956521739102</v>
       </c>
-      <c r="P25" s="10">
+      <c r="P28" s="10">
         <v>0.5</v>
       </c>
-      <c r="Q25" s="6">
+      <c r="Q28" s="6">
         <v>0.58333333333333304</v>
       </c>
-      <c r="R25" s="10">
+      <c r="R28" s="10">
         <v>0.58333333333333304</v>
       </c>
-      <c r="S25" s="10">
+      <c r="S28" s="10">
         <v>0.58333333333333304</v>
       </c>
-      <c r="T25" s="6">
+      <c r="T28" s="6">
         <v>0.4375</v>
       </c>
-      <c r="U25" s="10">
+      <c r="U28" s="10">
         <v>0.29166666666666602</v>
       </c>
-      <c r="V25" s="10">
+      <c r="V28" s="10">
         <v>0.5</v>
       </c>
-      <c r="W25" s="6">
+      <c r="W28" s="6">
         <v>0.46153846153846101</v>
       </c>
-      <c r="X25" s="10">
+      <c r="X28" s="10">
         <v>0.35294117647058798</v>
       </c>
-      <c r="Y25" s="10">
+      <c r="Y28" s="10">
         <v>0.5</v>
       </c>
-      <c r="Z25" s="6">
+      <c r="Z28" s="6">
         <v>0.37878787878787801</v>
       </c>
-      <c r="AA25" s="10">
+      <c r="AA28" s="10">
         <v>0.27777777777777701</v>
       </c>
-      <c r="AB25" s="10">
+      <c r="AB28" s="10">
         <v>0.41666666666666602</v>
       </c>
-      <c r="AC25" s="6">
+      <c r="AC28" s="6">
         <v>0.40983606557377</v>
       </c>
-      <c r="AD25" s="10">
+      <c r="AD28" s="10">
         <v>0.29411764705882298</v>
       </c>
-      <c r="AE25" s="24">
+      <c r="AE28" s="22">
         <v>0.45454545454545398</v>
       </c>
     </row>
-    <row r="26" spans="1:31" x14ac:dyDescent="0.35">
-      <c r="A26" s="3" t="s">
+    <row r="29" spans="1:32" x14ac:dyDescent="0.35">
+      <c r="A29" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="B26" s="6">
+      <c r="B29" s="6">
         <v>0</v>
       </c>
-      <c r="C26" s="10"/>
-      <c r="D26" s="10">
+      <c r="C29" s="10"/>
+      <c r="D29" s="10">
         <v>0</v>
       </c>
-      <c r="E26" s="6">
+      <c r="E29" s="6">
         <v>0</v>
       </c>
-      <c r="F26" s="10"/>
-      <c r="G26" s="10">
+      <c r="F29" s="10"/>
+      <c r="G29" s="10">
         <v>0</v>
       </c>
-      <c r="H26" s="6">
+      <c r="H29" s="6">
         <v>0</v>
       </c>
-      <c r="I26" s="10"/>
-      <c r="J26" s="10">
+      <c r="I29" s="10"/>
+      <c r="J29" s="10">
         <v>0</v>
       </c>
-      <c r="K26" s="6">
+      <c r="K29" s="6">
         <v>0</v>
       </c>
-      <c r="L26" s="10"/>
-      <c r="M26" s="10">
+      <c r="L29" s="10"/>
+      <c r="M29" s="10">
         <v>0</v>
       </c>
-      <c r="N26" s="6">
+      <c r="N29" s="6">
         <v>0</v>
       </c>
-      <c r="O26" s="10"/>
-      <c r="P26" s="10">
+      <c r="O29" s="10"/>
+      <c r="P29" s="10">
         <v>0</v>
       </c>
-      <c r="Q26" s="6">
+      <c r="Q29" s="6">
         <v>0</v>
       </c>
-      <c r="R26" s="10"/>
-      <c r="S26" s="10">
+      <c r="R29" s="10"/>
+      <c r="S29" s="10">
         <v>0</v>
       </c>
-      <c r="T26" s="6">
+      <c r="T29" s="6">
         <v>0</v>
       </c>
-      <c r="U26" s="10"/>
-      <c r="V26" s="10">
+      <c r="U29" s="10"/>
+      <c r="V29" s="10">
         <v>0</v>
       </c>
-      <c r="W26" s="6">
+      <c r="W29" s="6">
         <v>0</v>
       </c>
-      <c r="X26" s="10"/>
-      <c r="Y26" s="10">
+      <c r="X29" s="10"/>
+      <c r="Y29" s="10">
         <v>0</v>
       </c>
-      <c r="Z26" s="6">
+      <c r="Z29" s="6">
         <v>0</v>
       </c>
-      <c r="AA26" s="10"/>
-      <c r="AB26" s="10">
+      <c r="AA29" s="10"/>
+      <c r="AB29" s="10">
         <v>0</v>
       </c>
-      <c r="AC26" s="6">
+      <c r="AC29" s="6">
         <v>0</v>
       </c>
-      <c r="AD26" s="10"/>
-      <c r="AE26" s="24">
+      <c r="AD29" s="10"/>
+      <c r="AE29" s="22">
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:31" x14ac:dyDescent="0.35">
-      <c r="A27" s="3"/>
-      <c r="B27" s="6"/>
-      <c r="C27" s="10"/>
-      <c r="D27" s="10"/>
-      <c r="E27" s="6"/>
-      <c r="F27" s="10"/>
-      <c r="G27" s="10"/>
-      <c r="H27" s="6"/>
-      <c r="I27" s="10"/>
-      <c r="J27" s="10"/>
-      <c r="K27" s="6"/>
-      <c r="L27" s="10"/>
-      <c r="M27" s="10"/>
-      <c r="N27" s="6"/>
-      <c r="O27" s="10"/>
-      <c r="P27" s="10"/>
-      <c r="Q27" s="6"/>
-      <c r="R27" s="10"/>
-      <c r="S27" s="10"/>
-      <c r="T27" s="6"/>
-      <c r="U27" s="10"/>
-      <c r="V27" s="10"/>
-      <c r="W27" s="6"/>
-      <c r="X27" s="10"/>
-      <c r="Y27" s="10"/>
-      <c r="Z27" s="6"/>
-      <c r="AA27" s="10"/>
-      <c r="AB27" s="10"/>
-      <c r="AC27" s="6"/>
-      <c r="AD27" s="10"/>
-      <c r="AE27" s="24"/>
-    </row>
-    <row r="28" spans="1:31" x14ac:dyDescent="0.35">
-      <c r="A28" s="1" t="s">
+    <row r="30" spans="1:32" x14ac:dyDescent="0.35">
+      <c r="A30" s="3"/>
+      <c r="B30" s="6"/>
+      <c r="C30" s="10"/>
+      <c r="D30" s="10"/>
+      <c r="E30" s="6"/>
+      <c r="F30" s="10"/>
+      <c r="G30" s="10"/>
+      <c r="H30" s="6"/>
+      <c r="I30" s="10"/>
+      <c r="J30" s="10"/>
+      <c r="K30" s="6"/>
+      <c r="L30" s="10"/>
+      <c r="M30" s="10"/>
+      <c r="N30" s="6"/>
+      <c r="O30" s="10"/>
+      <c r="P30" s="10"/>
+      <c r="Q30" s="6"/>
+      <c r="R30" s="10"/>
+      <c r="S30" s="10"/>
+      <c r="T30" s="6"/>
+      <c r="U30" s="10"/>
+      <c r="V30" s="10"/>
+      <c r="W30" s="6"/>
+      <c r="X30" s="10"/>
+      <c r="Y30" s="10"/>
+      <c r="Z30" s="6"/>
+      <c r="AA30" s="10"/>
+      <c r="AB30" s="10"/>
+      <c r="AC30" s="6"/>
+      <c r="AD30" s="10"/>
+      <c r="AE30" s="22"/>
+    </row>
+    <row r="31" spans="1:32" x14ac:dyDescent="0.35">
+      <c r="A31" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="B28" s="7"/>
-      <c r="C28" s="11"/>
-      <c r="D28" s="8"/>
-      <c r="E28" s="7"/>
-      <c r="F28" s="11"/>
-      <c r="G28" s="8"/>
-      <c r="H28" s="7"/>
-      <c r="I28" s="11"/>
-      <c r="J28" s="8"/>
-      <c r="K28" s="7"/>
-      <c r="L28" s="11"/>
-      <c r="M28" s="11"/>
-      <c r="N28" s="7"/>
-      <c r="O28" s="11"/>
-      <c r="P28" s="11"/>
-      <c r="Q28" s="7"/>
-      <c r="R28" s="11"/>
-      <c r="S28" s="11"/>
-      <c r="T28" s="7"/>
-      <c r="U28" s="11"/>
-      <c r="V28" s="11"/>
-      <c r="W28" s="7"/>
-      <c r="X28" s="11"/>
-      <c r="Y28" s="11"/>
-      <c r="Z28" s="7"/>
-      <c r="AA28" s="11"/>
-      <c r="AB28" s="11"/>
-      <c r="AC28" s="7"/>
-      <c r="AD28" s="11"/>
-      <c r="AE28" s="8"/>
-    </row>
-    <row r="29" spans="1:31" x14ac:dyDescent="0.35">
-      <c r="A29" s="3" t="s">
+      <c r="B31" s="7"/>
+      <c r="C31" s="11"/>
+      <c r="D31" s="8"/>
+      <c r="E31" s="7"/>
+      <c r="F31" s="11"/>
+      <c r="G31" s="8"/>
+      <c r="H31" s="7"/>
+      <c r="I31" s="11"/>
+      <c r="J31" s="8"/>
+      <c r="K31" s="7"/>
+      <c r="L31" s="11"/>
+      <c r="M31" s="11"/>
+      <c r="N31" s="7"/>
+      <c r="O31" s="11"/>
+      <c r="P31" s="11"/>
+      <c r="Q31" s="7"/>
+      <c r="R31" s="11"/>
+      <c r="S31" s="11"/>
+      <c r="T31" s="7"/>
+      <c r="U31" s="11"/>
+      <c r="V31" s="11"/>
+      <c r="W31" s="7"/>
+      <c r="X31" s="11"/>
+      <c r="Y31" s="11"/>
+      <c r="Z31" s="7"/>
+      <c r="AA31" s="11"/>
+      <c r="AB31" s="11"/>
+      <c r="AC31" s="7"/>
+      <c r="AD31" s="11"/>
+      <c r="AE31" s="8"/>
+    </row>
+    <row r="32" spans="1:32" x14ac:dyDescent="0.35">
+      <c r="A32" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="B29" s="6">
+      <c r="B32" s="6">
         <v>0.55147058823529405</v>
       </c>
-      <c r="C29" s="10">
+      <c r="C32" s="10">
         <v>0.234375</v>
       </c>
-      <c r="D29" s="10">
+      <c r="D32" s="10">
         <v>0.83333333333333304</v>
       </c>
-      <c r="E29" s="6">
+      <c r="E32" s="6">
         <v>0.53435114503816705</v>
       </c>
-      <c r="F29" s="10">
+      <c r="F32" s="10">
         <v>0.22222222222222199</v>
       </c>
-      <c r="G29" s="10">
+      <c r="G32" s="10">
         <v>0.82352941176470495</v>
       </c>
-      <c r="H29" s="6">
+      <c r="H32" s="6">
         <v>0.53846153846153799</v>
       </c>
-      <c r="I29" s="10">
+      <c r="I32" s="10">
         <v>0.225806451612903</v>
       </c>
-      <c r="J29" s="10">
+      <c r="J32" s="10">
         <v>0.82352941176470495</v>
       </c>
-      <c r="K29" s="6">
+      <c r="K32" s="6">
         <v>0.50724637681159401</v>
       </c>
-      <c r="L29" s="10">
+      <c r="L32" s="10">
         <v>0.2</v>
       </c>
-      <c r="M29" s="10">
+      <c r="M32" s="10">
         <v>0.82352941176470495</v>
       </c>
-      <c r="N29" s="6">
+      <c r="N32" s="6">
         <v>0.59748427672955895</v>
       </c>
-      <c r="O29" s="10">
+      <c r="O32" s="10">
         <v>0.26760563380281599</v>
       </c>
-      <c r="P29" s="10">
+      <c r="P32" s="10">
         <v>0.86363636363636298</v>
       </c>
-      <c r="Q29" s="6">
+      <c r="Q32" s="6">
         <v>0.53435114503816705</v>
       </c>
-      <c r="R29" s="10">
+      <c r="R32" s="10">
         <v>0.22222222222222199</v>
       </c>
-      <c r="S29" s="10">
+      <c r="S32" s="10">
         <v>0.82352941176470495</v>
       </c>
-      <c r="T29" s="6">
+      <c r="T32" s="6">
         <v>0.53435114503816705</v>
       </c>
-      <c r="U29" s="10">
+      <c r="U32" s="10">
         <v>0.22222222222222199</v>
       </c>
-      <c r="V29" s="10">
+      <c r="V32" s="10">
         <v>0.82352941176470495</v>
       </c>
-      <c r="W29" s="6">
+      <c r="W32" s="6">
         <v>0.59027777777777701</v>
       </c>
-      <c r="X29" s="10">
+      <c r="X32" s="10">
         <v>0.25</v>
       </c>
-      <c r="Y29" s="10">
+      <c r="Y32" s="10">
         <v>0.89473684210526305</v>
       </c>
-      <c r="Z29" s="6">
+      <c r="Z32" s="6">
         <v>0.48148148148148101</v>
       </c>
-      <c r="AA29" s="10">
+      <c r="AA32" s="10">
         <v>0.194029850746268</v>
       </c>
-      <c r="AB29" s="10">
+      <c r="AB32" s="10">
         <v>0.76470588235294101</v>
       </c>
-      <c r="AC29" s="6">
+      <c r="AC32" s="6">
         <v>0.44715447154471499</v>
       </c>
-      <c r="AD29" s="10">
+      <c r="AD32" s="10">
         <v>0.17460317460317401</v>
       </c>
-      <c r="AE29" s="24">
+      <c r="AE32" s="22">
         <v>0.73333333333333295</v>
       </c>
     </row>
-    <row r="30" spans="1:31" x14ac:dyDescent="0.35">
-      <c r="A30" s="16" t="s">
+    <row r="33" spans="1:31" x14ac:dyDescent="0.35">
+      <c r="A33" s="15" t="s">
         <v>29</v>
       </c>
-      <c r="B30" s="14">
+      <c r="B33" s="13">
         <v>0.62992125984251901</v>
       </c>
-      <c r="C30" s="15">
+      <c r="C33" s="14">
         <v>0.29090909090909001</v>
       </c>
-      <c r="D30" s="15">
+      <c r="D33" s="14">
         <v>0.88888888888888795</v>
       </c>
-      <c r="E30" s="14">
+      <c r="E33" s="13">
         <v>0.62992125984251901</v>
       </c>
-      <c r="F30" s="15">
+      <c r="F33" s="14">
         <v>0.31372549019607798</v>
       </c>
-      <c r="G30" s="15">
+      <c r="G33" s="14">
         <v>0.84210526315789402</v>
       </c>
-      <c r="H30" s="14">
+      <c r="H33" s="13">
         <v>0.57851239669421395</v>
       </c>
-      <c r="I30" s="15">
+      <c r="I33" s="14">
         <v>0.26415094339622602</v>
       </c>
-      <c r="J30" s="15">
+      <c r="J33" s="14">
         <v>0.82352941176470495</v>
       </c>
-      <c r="K30" s="14">
+      <c r="K33" s="13">
         <v>0.47297297297297303</v>
       </c>
-      <c r="L30" s="15">
+      <c r="L33" s="14">
         <v>0.18421052631578899</v>
       </c>
-      <c r="M30" s="15">
+      <c r="M33" s="14">
         <v>0.77777777777777701</v>
       </c>
-      <c r="N30" s="14">
+      <c r="N33" s="13">
         <v>0.54263565891472798</v>
       </c>
-      <c r="O30" s="15">
+      <c r="O33" s="14">
         <v>0.24561403508771901</v>
       </c>
-      <c r="P30" s="15">
+      <c r="P33" s="14">
         <v>0.77777777777777701</v>
       </c>
-      <c r="Q30" s="14">
+      <c r="Q33" s="13">
         <v>0.61403508771929804</v>
       </c>
-      <c r="R30" s="15">
+      <c r="R33" s="14">
         <v>0.28000000000000003</v>
       </c>
-      <c r="S30" s="15">
+      <c r="S33" s="14">
         <v>0.875</v>
       </c>
-      <c r="T30" s="14">
+      <c r="T33" s="13">
         <v>0.58823529411764697</v>
       </c>
-      <c r="U30" s="15">
+      <c r="U33" s="14">
         <v>0.27450980392156799</v>
       </c>
-      <c r="V30" s="15">
+      <c r="V33" s="14">
         <v>0.82352941176470495</v>
       </c>
-      <c r="W30" s="14">
+      <c r="W33" s="13">
         <v>0.592592592592592</v>
       </c>
-      <c r="X30" s="15">
+      <c r="X33" s="14">
         <v>0.25396825396825301</v>
       </c>
-      <c r="Y30" s="15">
+      <c r="Y33" s="14">
         <v>0.88888888888888795</v>
       </c>
-      <c r="Z30" s="14">
+      <c r="Z33" s="13">
         <v>0.54166666666666596</v>
       </c>
-      <c r="AA30" s="15">
+      <c r="AA33" s="14">
         <v>0.23214285714285701</v>
       </c>
-      <c r="AB30" s="15">
+      <c r="AB33" s="14">
         <v>0.8125</v>
       </c>
-      <c r="AC30" s="14">
+      <c r="AC33" s="13">
         <v>0.61224489795918302</v>
       </c>
-      <c r="AD30" s="15">
+      <c r="AD33" s="14">
         <v>0.26865671641791</v>
       </c>
-      <c r="AE30" s="23">
+      <c r="AE33" s="21">
         <v>0.9</v>
       </c>
-    </row>
-    <row r="31" spans="1:31" x14ac:dyDescent="0.35">
-      <c r="A31" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="B31" s="6">
-        <v>0.47297297297297303</v>
-      </c>
-      <c r="C31" s="10">
-        <v>0.31818181818181801</v>
-      </c>
-      <c r="D31" s="10">
-        <v>0.53846153846153799</v>
-      </c>
-      <c r="E31" s="6">
-        <v>0.434782608695652</v>
-      </c>
-      <c r="F31" s="10">
-        <v>0.28571428571428498</v>
-      </c>
-      <c r="G31" s="10">
-        <v>0.5</v>
-      </c>
-      <c r="H31" s="6">
-        <v>0.47297297297297303</v>
-      </c>
-      <c r="I31" s="10">
-        <v>0.31818181818181801</v>
-      </c>
-      <c r="J31" s="10">
-        <v>0.53846153846153799</v>
-      </c>
-      <c r="K31" s="6">
-        <v>0.394736842105263</v>
-      </c>
-      <c r="L31" s="10">
-        <v>0.16666666666666599</v>
-      </c>
-      <c r="M31" s="10">
-        <v>0.6</v>
-      </c>
-      <c r="N31" s="6">
-        <v>0.36842105263157798</v>
-      </c>
-      <c r="O31" s="10">
-        <v>0.16279069767441801</v>
-      </c>
-      <c r="P31" s="10">
-        <v>0.53846153846153799</v>
-      </c>
-      <c r="Q31" s="6">
-        <v>0.41666666666666602</v>
-      </c>
-      <c r="R31" s="10">
-        <v>0.25</v>
-      </c>
-      <c r="S31" s="10">
-        <v>0.5</v>
-      </c>
-      <c r="T31" s="6">
-        <v>0.21126760563380201</v>
-      </c>
-      <c r="U31" s="10">
-        <v>0.11111111111111099</v>
-      </c>
-      <c r="V31" s="10">
-        <v>0.27272727272727199</v>
-      </c>
-      <c r="W31" s="6">
-        <v>0.34722222222222199</v>
-      </c>
-      <c r="X31" s="10">
-        <v>0.17857142857142799</v>
-      </c>
-      <c r="Y31" s="10">
-        <v>0.45454545454545398</v>
-      </c>
-      <c r="Z31" s="6">
-        <v>0.42682926829268197</v>
-      </c>
-      <c r="AA31" s="10">
-        <v>0.233333333333333</v>
-      </c>
-      <c r="AB31" s="10">
-        <v>0.53846153846153799</v>
-      </c>
-      <c r="AC31" s="6">
-        <v>0.34722222222222199</v>
-      </c>
-      <c r="AD31" s="10">
-        <v>0.20833333333333301</v>
-      </c>
-      <c r="AE31" s="24">
-        <v>0.41666666666666602</v>
-      </c>
-    </row>
-    <row r="32" spans="1:31" x14ac:dyDescent="0.35">
-      <c r="A32" s="3"/>
-      <c r="B32" s="6"/>
-      <c r="C32" s="10"/>
-      <c r="D32" s="10"/>
-      <c r="E32" s="6"/>
-      <c r="F32" s="10"/>
-      <c r="G32" s="10"/>
-      <c r="H32" s="6"/>
-      <c r="I32" s="10"/>
-      <c r="J32" s="10"/>
-      <c r="K32" s="6"/>
-      <c r="L32" s="10"/>
-      <c r="M32" s="10"/>
-      <c r="N32" s="6"/>
-      <c r="O32" s="10"/>
-      <c r="P32" s="10"/>
-      <c r="Q32" s="6"/>
-      <c r="R32" s="10"/>
-      <c r="S32" s="10"/>
-      <c r="T32" s="6"/>
-      <c r="U32" s="10"/>
-      <c r="V32" s="10"/>
-      <c r="W32" s="6"/>
-      <c r="X32" s="10"/>
-      <c r="Y32" s="10"/>
-      <c r="Z32" s="6"/>
-      <c r="AA32" s="10"/>
-      <c r="AB32" s="10"/>
-      <c r="AC32" s="6"/>
-      <c r="AD32" s="10"/>
-      <c r="AE32" s="24"/>
-    </row>
-    <row r="33" spans="1:31" x14ac:dyDescent="0.35">
-      <c r="A33" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="B33" s="7"/>
-      <c r="C33" s="11"/>
-      <c r="D33" s="8"/>
-      <c r="E33" s="7"/>
-      <c r="F33" s="11"/>
-      <c r="G33" s="8"/>
-      <c r="H33" s="7"/>
-      <c r="I33" s="11"/>
-      <c r="J33" s="8"/>
-      <c r="K33" s="7"/>
-      <c r="L33" s="11"/>
-      <c r="M33" s="11"/>
-      <c r="N33" s="7"/>
-      <c r="O33" s="11"/>
-      <c r="P33" s="11"/>
-      <c r="Q33" s="7"/>
-      <c r="R33" s="11"/>
-      <c r="S33" s="11"/>
-      <c r="T33" s="7"/>
-      <c r="U33" s="11"/>
-      <c r="V33" s="11"/>
-      <c r="W33" s="7"/>
-      <c r="X33" s="11"/>
-      <c r="Y33" s="11"/>
-      <c r="Z33" s="7"/>
-      <c r="AA33" s="11"/>
-      <c r="AB33" s="11"/>
-      <c r="AC33" s="7"/>
-      <c r="AD33" s="11"/>
-      <c r="AE33" s="8"/>
     </row>
     <row r="34" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A34" s="3" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="B34" s="6">
-        <v>8.3333333333333301E-2</v>
+        <v>0.47297297297297303</v>
       </c>
       <c r="C34" s="10">
-        <v>0.05</v>
+        <v>0.31818181818181801</v>
       </c>
       <c r="D34" s="10">
-        <v>0.1</v>
+        <v>0.53846153846153799</v>
       </c>
       <c r="E34" s="6">
-        <v>0.30303030303030298</v>
+        <v>0.434782608695652</v>
       </c>
       <c r="F34" s="10">
-        <v>0.18181818181818099</v>
+        <v>0.28571428571428498</v>
       </c>
       <c r="G34" s="10">
-        <v>0.36363636363636298</v>
+        <v>0.5</v>
       </c>
       <c r="H34" s="6">
-        <v>0.37313432835820898</v>
+        <v>0.47297297297297303</v>
       </c>
       <c r="I34" s="10">
-        <v>0.217391304347826</v>
+        <v>0.31818181818181801</v>
       </c>
       <c r="J34" s="10">
-        <v>0.45454545454545398</v>
+        <v>0.53846153846153799</v>
       </c>
       <c r="K34" s="6">
-        <v>0.43859649122806998</v>
+        <v>0.394736842105263</v>
       </c>
       <c r="L34" s="10">
-        <v>0.18518518518518501</v>
+        <v>0.16666666666666599</v>
       </c>
       <c r="M34" s="10">
-        <v>0.66666666666666596</v>
+        <v>0.6</v>
       </c>
       <c r="N34" s="6">
-        <v>0.30864197530864201</v>
+        <v>0.36842105263157798</v>
       </c>
       <c r="O34" s="10">
-        <v>0.15151515151515099</v>
+        <v>0.16279069767441801</v>
       </c>
       <c r="P34" s="10">
+        <v>0.53846153846153799</v>
+      </c>
+      <c r="Q34" s="6">
         <v>0.41666666666666602</v>
       </c>
-      <c r="Q34" s="6">
-        <v>0.22388059701492499</v>
-      </c>
       <c r="R34" s="10">
-        <v>0.13043478260869501</v>
+        <v>0.25</v>
       </c>
       <c r="S34" s="10">
+        <v>0.5</v>
+      </c>
+      <c r="T34" s="6">
+        <v>0.21126760563380201</v>
+      </c>
+      <c r="U34" s="10">
+        <v>0.11111111111111099</v>
+      </c>
+      <c r="V34" s="10">
         <v>0.27272727272727199</v>
-      </c>
-      <c r="T34" s="6">
-        <v>0.33333333333333298</v>
-      </c>
-      <c r="U34" s="10">
-        <v>0.16129032258064499</v>
-      </c>
-      <c r="V34" s="10">
-        <v>0.45454545454545398</v>
       </c>
       <c r="W34" s="6">
         <v>0.34722222222222199</v>
       </c>
       <c r="X34" s="10">
+        <v>0.17857142857142799</v>
+      </c>
+      <c r="Y34" s="10">
+        <v>0.45454545454545398</v>
+      </c>
+      <c r="Z34" s="6">
+        <v>0.42682926829268197</v>
+      </c>
+      <c r="AA34" s="10">
+        <v>0.233333333333333</v>
+      </c>
+      <c r="AB34" s="10">
+        <v>0.53846153846153799</v>
+      </c>
+      <c r="AC34" s="6">
+        <v>0.34722222222222199</v>
+      </c>
+      <c r="AD34" s="10">
         <v>0.20833333333333301</v>
       </c>
-      <c r="Y34" s="10">
+      <c r="AE34" s="22">
         <v>0.41666666666666602</v>
       </c>
-      <c r="Z34" s="6">
+    </row>
+    <row r="35" spans="1:31" x14ac:dyDescent="0.35">
+      <c r="A35" s="3"/>
+      <c r="B35" s="6"/>
+      <c r="C35" s="10"/>
+      <c r="D35" s="10"/>
+      <c r="E35" s="6"/>
+      <c r="F35" s="10"/>
+      <c r="G35" s="10"/>
+      <c r="H35" s="6"/>
+      <c r="I35" s="10"/>
+      <c r="J35" s="10"/>
+      <c r="K35" s="6"/>
+      <c r="L35" s="10"/>
+      <c r="M35" s="10"/>
+      <c r="N35" s="6"/>
+      <c r="O35" s="10"/>
+      <c r="P35" s="10"/>
+      <c r="Q35" s="6"/>
+      <c r="R35" s="10"/>
+      <c r="S35" s="10"/>
+      <c r="T35" s="6"/>
+      <c r="U35" s="10"/>
+      <c r="V35" s="10"/>
+      <c r="W35" s="6"/>
+      <c r="X35" s="10"/>
+      <c r="Y35" s="10"/>
+      <c r="Z35" s="6"/>
+      <c r="AA35" s="10"/>
+      <c r="AB35" s="10"/>
+      <c r="AC35" s="6"/>
+      <c r="AD35" s="10"/>
+      <c r="AE35" s="22"/>
+    </row>
+    <row r="36" spans="1:31" x14ac:dyDescent="0.35">
+      <c r="A36" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B36" s="7"/>
+      <c r="C36" s="11"/>
+      <c r="D36" s="8"/>
+      <c r="E36" s="7"/>
+      <c r="F36" s="11"/>
+      <c r="G36" s="8"/>
+      <c r="H36" s="7"/>
+      <c r="I36" s="11"/>
+      <c r="J36" s="8"/>
+      <c r="K36" s="7"/>
+      <c r="L36" s="11"/>
+      <c r="M36" s="11"/>
+      <c r="N36" s="7"/>
+      <c r="O36" s="11"/>
+      <c r="P36" s="11"/>
+      <c r="Q36" s="7"/>
+      <c r="R36" s="11"/>
+      <c r="S36" s="11"/>
+      <c r="T36" s="7"/>
+      <c r="U36" s="11"/>
+      <c r="V36" s="11"/>
+      <c r="W36" s="7"/>
+      <c r="X36" s="11"/>
+      <c r="Y36" s="11"/>
+      <c r="Z36" s="7"/>
+      <c r="AA36" s="11"/>
+      <c r="AB36" s="11"/>
+      <c r="AC36" s="7"/>
+      <c r="AD36" s="11"/>
+      <c r="AE36" s="8"/>
+    </row>
+    <row r="37" spans="1:31" x14ac:dyDescent="0.35">
+      <c r="A37" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="B37" s="6">
+        <v>8.3333333333333301E-2</v>
+      </c>
+      <c r="C37" s="10">
+        <v>0.05</v>
+      </c>
+      <c r="D37" s="10">
+        <v>0.1</v>
+      </c>
+      <c r="E37" s="6">
+        <v>0.30303030303030298</v>
+      </c>
+      <c r="F37" s="10">
+        <v>0.18181818181818099</v>
+      </c>
+      <c r="G37" s="10">
+        <v>0.36363636363636298</v>
+      </c>
+      <c r="H37" s="6">
+        <v>0.37313432835820898</v>
+      </c>
+      <c r="I37" s="10">
+        <v>0.217391304347826</v>
+      </c>
+      <c r="J37" s="10">
+        <v>0.45454545454545398</v>
+      </c>
+      <c r="K37" s="6">
+        <v>0.43859649122806998</v>
+      </c>
+      <c r="L37" s="10">
+        <v>0.18518518518518501</v>
+      </c>
+      <c r="M37" s="10">
+        <v>0.66666666666666596</v>
+      </c>
+      <c r="N37" s="6">
+        <v>0.30864197530864201</v>
+      </c>
+      <c r="O37" s="10">
+        <v>0.15151515151515099</v>
+      </c>
+      <c r="P37" s="10">
+        <v>0.41666666666666602</v>
+      </c>
+      <c r="Q37" s="6">
+        <v>0.22388059701492499</v>
+      </c>
+      <c r="R37" s="10">
+        <v>0.13043478260869501</v>
+      </c>
+      <c r="S37" s="10">
+        <v>0.27272727272727199</v>
+      </c>
+      <c r="T37" s="6">
         <v>0.33333333333333298</v>
       </c>
-      <c r="AA34" s="10">
+      <c r="U37" s="10">
         <v>0.16129032258064499</v>
       </c>
-      <c r="AB34" s="10">
+      <c r="V37" s="10">
         <v>0.45454545454545398</v>
       </c>
-      <c r="AC34" s="6">
+      <c r="W37" s="6">
+        <v>0.34722222222222199</v>
+      </c>
+      <c r="X37" s="10">
+        <v>0.20833333333333301</v>
+      </c>
+      <c r="Y37" s="10">
+        <v>0.41666666666666602</v>
+      </c>
+      <c r="Z37" s="6">
+        <v>0.33333333333333298</v>
+      </c>
+      <c r="AA37" s="10">
+        <v>0.16129032258064499</v>
+      </c>
+      <c r="AB37" s="10">
+        <v>0.45454545454545398</v>
+      </c>
+      <c r="AC37" s="6">
         <v>0.32051282051281998</v>
       </c>
-      <c r="AD34" s="10">
+      <c r="AD37" s="10">
         <v>0.16666666666666599</v>
       </c>
-      <c r="AE34" s="24">
+      <c r="AE37" s="22">
         <v>0.41666666666666602</v>
       </c>
     </row>
-    <row r="35" spans="1:31" x14ac:dyDescent="0.35">
-      <c r="A35" s="3" t="s">
+    <row r="38" spans="1:31" x14ac:dyDescent="0.35">
+      <c r="A38" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="B35" s="6">
+      <c r="B38" s="6">
         <v>0.38461538461538403</v>
       </c>
-      <c r="C35" s="10">
+      <c r="C38" s="10">
         <v>0.33333333333333298</v>
       </c>
-      <c r="D35" s="10">
+      <c r="D38" s="10">
         <v>0.4</v>
       </c>
-      <c r="E35" s="6">
+      <c r="E38" s="6">
         <v>0.3125</v>
       </c>
-      <c r="F35" s="10">
+      <c r="F38" s="10">
         <v>0.375</v>
       </c>
-      <c r="G35" s="10">
+      <c r="G38" s="10">
         <v>0.3</v>
       </c>
-      <c r="H35" s="6">
+      <c r="H38" s="6">
         <v>9.8039215686274495E-2</v>
       </c>
-      <c r="I35" s="10">
+      <c r="I38" s="10">
         <v>9.0909090909090898E-2</v>
       </c>
-      <c r="J35" s="10">
+      <c r="J38" s="10">
         <v>0.1</v>
       </c>
-      <c r="K35" s="6">
+      <c r="K38" s="6">
         <v>0.476190476190476</v>
       </c>
-      <c r="L35" s="10">
+      <c r="L38" s="10">
         <v>0.24390243902438999</v>
       </c>
-      <c r="M35" s="10">
+      <c r="M38" s="10">
         <v>0.625</v>
       </c>
-      <c r="N35" s="6">
+      <c r="N38" s="6">
         <v>0.52631578947368396</v>
       </c>
-      <c r="O35" s="10">
+      <c r="O38" s="10">
         <v>0.33333333333333298</v>
       </c>
-      <c r="P35" s="10">
+      <c r="P38" s="10">
         <v>0.61538461538461497</v>
       </c>
-      <c r="Q35" s="6">
+      <c r="Q38" s="6">
         <v>0.38461538461538403</v>
       </c>
-      <c r="R35" s="10">
+      <c r="R38" s="10">
         <v>0.33333333333333298</v>
       </c>
-      <c r="S35" s="10">
+      <c r="S38" s="10">
         <v>0.4</v>
       </c>
-      <c r="T35" s="6">
+      <c r="T38" s="6">
         <v>0.45454545454545398</v>
       </c>
-      <c r="U35" s="10">
+      <c r="U38" s="10">
         <v>0.42857142857142799</v>
       </c>
-      <c r="V35" s="10">
+      <c r="V38" s="10">
         <v>0.46153846153846101</v>
       </c>
-      <c r="W35" s="6">
+      <c r="W38" s="6">
         <v>0.46875</v>
       </c>
-      <c r="X35" s="10">
+      <c r="X38" s="10">
         <v>0.3</v>
       </c>
-      <c r="Y35" s="10">
+      <c r="Y38" s="10">
         <v>0.54545454545454497</v>
       </c>
-      <c r="Z35" s="6">
+      <c r="Z38" s="6">
         <v>0.30303030303030298</v>
       </c>
-      <c r="AA35" s="10">
+      <c r="AA38" s="10">
         <v>0.18181818181818099</v>
       </c>
-      <c r="AB35" s="10">
+      <c r="AB38" s="10">
         <v>0.36363636363636298</v>
       </c>
-      <c r="AC35" s="6">
+      <c r="AC38" s="6">
         <v>0.34722222222222199</v>
       </c>
-      <c r="AD35" s="10">
+      <c r="AD38" s="10">
         <v>0.20833333333333301</v>
       </c>
-      <c r="AE35" s="24">
+      <c r="AE38" s="22">
         <v>0.41666666666666602</v>
       </c>
     </row>
-    <row r="36" spans="1:31" x14ac:dyDescent="0.35">
-      <c r="A36" s="3" t="s">
+    <row r="39" spans="1:31" x14ac:dyDescent="0.35">
+      <c r="A39" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="B36" s="6">
+      <c r="B39" s="6">
         <v>0.116279069767441</v>
       </c>
-      <c r="C36" s="10">
+      <c r="C39" s="10">
         <v>0.33333333333333298</v>
       </c>
-      <c r="D36" s="10">
+      <c r="D39" s="10">
         <v>0.1</v>
       </c>
-      <c r="E36" s="6">
+      <c r="E39" s="6">
         <v>0.116279069767441</v>
       </c>
-      <c r="F36" s="10">
+      <c r="F39" s="10">
         <v>0.33333333333333298</v>
       </c>
-      <c r="G36" s="10">
+      <c r="G39" s="10">
         <v>0.1</v>
       </c>
-      <c r="H36" s="6">
+      <c r="H39" s="6">
         <v>0</v>
       </c>
-      <c r="I36" s="10">
+      <c r="I39" s="10">
         <v>0</v>
       </c>
-      <c r="J36" s="10">
+      <c r="J39" s="10">
         <v>0</v>
       </c>
-      <c r="K36" s="6">
+      <c r="K39" s="6">
         <v>0.20408163265306101</v>
       </c>
-      <c r="L36" s="10">
+      <c r="L39" s="10">
         <v>0.22222222222222199</v>
       </c>
-      <c r="M36" s="10">
+      <c r="M39" s="10">
         <v>0.2</v>
       </c>
-      <c r="N36" s="6">
+      <c r="N39" s="6">
         <v>0.3125</v>
       </c>
-      <c r="O36" s="10">
+      <c r="O39" s="10">
         <v>0.75</v>
       </c>
-      <c r="P36" s="10">
+      <c r="P39" s="10">
         <v>0.27272727272727199</v>
       </c>
-      <c r="Q36" s="6">
+      <c r="Q39" s="6">
         <v>0.11363636363636299</v>
       </c>
-      <c r="R36" s="10">
+      <c r="R39" s="10">
         <v>0.25</v>
       </c>
-      <c r="S36" s="10">
+      <c r="S39" s="10">
         <v>0.1</v>
       </c>
-      <c r="T36" s="6">
+      <c r="T39" s="6">
         <v>0.11111111111111099</v>
       </c>
-      <c r="U36" s="10">
+      <c r="U39" s="10">
         <v>0.2</v>
       </c>
-      <c r="V36" s="10">
+      <c r="V39" s="10">
         <v>0.1</v>
       </c>
-      <c r="W36" s="6">
+      <c r="W39" s="6">
         <v>0.29411764705882298</v>
       </c>
-      <c r="X36" s="10">
+      <c r="X39" s="10">
         <v>0.42857142857142799</v>
       </c>
-      <c r="Y36" s="10">
+      <c r="Y39" s="10">
         <v>0.27272727272727199</v>
       </c>
-      <c r="Z36" s="6">
+      <c r="Z39" s="6">
         <v>0.19607843137254899</v>
       </c>
-      <c r="AA36" s="10">
+      <c r="AA39" s="10">
         <v>0.28571428571428498</v>
       </c>
-      <c r="AB36" s="10">
+      <c r="AB39" s="10">
         <v>0.18181818181818099</v>
       </c>
-      <c r="AC36" s="6">
+      <c r="AC39" s="6">
         <v>0.22222222222222199</v>
       </c>
-      <c r="AD36" s="10">
+      <c r="AD39" s="10">
         <v>0.4</v>
       </c>
-      <c r="AE36" s="24">
+      <c r="AE39" s="22">
         <v>0.2</v>
       </c>
     </row>
-    <row r="37" spans="1:31" x14ac:dyDescent="0.35">
-      <c r="A37" s="16" t="s">
+    <row r="40" spans="1:31" x14ac:dyDescent="0.35">
+      <c r="A40" s="15" t="s">
         <v>36</v>
       </c>
-      <c r="B37" s="14">
+      <c r="B40" s="13">
         <v>0.60747663551401798</v>
       </c>
-      <c r="C37" s="15">
+      <c r="C40" s="14">
         <v>0.33333333333333298</v>
       </c>
-      <c r="D37" s="15">
+      <c r="D40" s="14">
         <v>0.76470588235294101</v>
       </c>
-      <c r="E37" s="14">
+      <c r="E40" s="13">
         <v>0.660377358490566</v>
       </c>
-      <c r="F37" s="15">
+      <c r="F40" s="14">
         <v>0.41176470588235198</v>
       </c>
-      <c r="G37" s="15">
+      <c r="G40" s="14">
         <v>0.77777777777777701</v>
       </c>
-      <c r="H37" s="14">
+      <c r="H40" s="13">
         <v>0.68627450980392102</v>
       </c>
-      <c r="I37" s="15">
+      <c r="I40" s="14">
         <v>0.41176470588235198</v>
       </c>
-      <c r="J37" s="15">
+      <c r="J40" s="14">
         <v>0.82352941176470495</v>
       </c>
-      <c r="K37" s="14">
+      <c r="K40" s="13">
         <v>0.58064516129032195</v>
       </c>
-      <c r="L37" s="15">
+      <c r="L40" s="14">
         <v>0.24</v>
       </c>
-      <c r="M37" s="15">
+      <c r="M40" s="14">
         <v>0.9</v>
       </c>
-      <c r="N37" s="14">
+      <c r="N40" s="13">
         <v>0.57251908396946505</v>
       </c>
-      <c r="O37" s="15">
+      <c r="O40" s="14">
         <v>0.27272727272727199</v>
       </c>
-      <c r="P37" s="15">
+      <c r="P40" s="14">
         <v>0.78947368421052599</v>
       </c>
-      <c r="Q37" s="14">
+      <c r="Q40" s="13">
         <v>0.63636363636363602</v>
       </c>
-      <c r="R37" s="15">
+      <c r="R40" s="14">
         <v>0.33333333333333298</v>
       </c>
-      <c r="S37" s="15">
+      <c r="S40" s="14">
         <v>0.82352941176470495</v>
       </c>
-      <c r="T37" s="14">
+      <c r="T40" s="13">
         <v>0.66371681415929196</v>
       </c>
-      <c r="U37" s="15">
+      <c r="U40" s="14">
         <v>0.33333333333333298</v>
       </c>
-      <c r="V37" s="15">
+      <c r="V40" s="14">
         <v>0.88235294117647001</v>
       </c>
-      <c r="W37" s="14">
+      <c r="W40" s="13">
         <v>0.64102564102564097</v>
       </c>
-      <c r="X37" s="15">
+      <c r="X40" s="14">
         <v>0.30612244897959101</v>
       </c>
-      <c r="Y37" s="15">
+      <c r="Y40" s="14">
         <v>0.88235294117647001</v>
       </c>
-      <c r="Z37" s="14">
+      <c r="Z40" s="13">
         <v>0.61904761904761896</v>
       </c>
-      <c r="AA37" s="15">
+      <c r="AA40" s="14">
         <v>0.31707317073170699</v>
       </c>
-      <c r="AB37" s="15">
+      <c r="AB40" s="14">
         <v>0.8125</v>
       </c>
-      <c r="AC37" s="14">
+      <c r="AC40" s="13">
         <v>0.64</v>
       </c>
-      <c r="AD37" s="15">
+      <c r="AD40" s="14">
         <v>0.32653061224489699</v>
       </c>
-      <c r="AE37" s="23">
+      <c r="AE40" s="21">
         <v>0.84210526315789402</v>
       </c>
     </row>
-    <row r="38" spans="1:31" x14ac:dyDescent="0.35">
-      <c r="A38" s="3"/>
-      <c r="B38" s="6"/>
-      <c r="C38" s="10"/>
-      <c r="D38" s="10"/>
-      <c r="E38" s="6"/>
-      <c r="F38" s="10"/>
-      <c r="G38" s="10"/>
-      <c r="H38" s="6"/>
-      <c r="I38" s="10"/>
-      <c r="J38" s="10"/>
-      <c r="K38" s="6"/>
-      <c r="L38" s="10"/>
-      <c r="M38" s="10"/>
-      <c r="N38" s="6"/>
-      <c r="O38" s="10"/>
-      <c r="P38" s="10"/>
-      <c r="Q38" s="6"/>
-      <c r="R38" s="10"/>
-      <c r="S38" s="10"/>
-      <c r="T38" s="6"/>
-      <c r="U38" s="10"/>
-      <c r="V38" s="10"/>
-      <c r="W38" s="6"/>
-      <c r="X38" s="10"/>
-      <c r="Y38" s="10"/>
-      <c r="Z38" s="6"/>
-      <c r="AA38" s="10"/>
-      <c r="AB38" s="10"/>
-      <c r="AC38" s="6"/>
-      <c r="AD38" s="10"/>
-      <c r="AE38" s="24"/>
-    </row>
-    <row r="39" spans="1:31" x14ac:dyDescent="0.35">
-      <c r="A39" s="1" t="s">
+    <row r="41" spans="1:31" x14ac:dyDescent="0.35">
+      <c r="A41" s="3"/>
+      <c r="B41" s="6"/>
+      <c r="C41" s="10"/>
+      <c r="D41" s="10"/>
+      <c r="E41" s="6"/>
+      <c r="F41" s="10"/>
+      <c r="G41" s="10"/>
+      <c r="H41" s="6"/>
+      <c r="I41" s="10"/>
+      <c r="J41" s="10"/>
+      <c r="K41" s="6"/>
+      <c r="L41" s="10"/>
+      <c r="M41" s="10"/>
+      <c r="N41" s="6"/>
+      <c r="O41" s="10"/>
+      <c r="P41" s="10"/>
+      <c r="Q41" s="6"/>
+      <c r="R41" s="10"/>
+      <c r="S41" s="10"/>
+      <c r="T41" s="6"/>
+      <c r="U41" s="10"/>
+      <c r="V41" s="10"/>
+      <c r="W41" s="6"/>
+      <c r="X41" s="10"/>
+      <c r="Y41" s="10"/>
+      <c r="Z41" s="6"/>
+      <c r="AA41" s="10"/>
+      <c r="AB41" s="10"/>
+      <c r="AC41" s="6"/>
+      <c r="AD41" s="10"/>
+      <c r="AE41" s="22"/>
+    </row>
+    <row r="42" spans="1:31" x14ac:dyDescent="0.35">
+      <c r="A42" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="B39" s="7"/>
-      <c r="C39" s="11"/>
-      <c r="D39" s="8"/>
-      <c r="E39" s="7"/>
-      <c r="F39" s="11"/>
-      <c r="G39" s="8"/>
-      <c r="H39" s="7"/>
-      <c r="I39" s="11"/>
-      <c r="J39" s="8"/>
-      <c r="K39" s="7"/>
-      <c r="L39" s="11"/>
-      <c r="M39" s="11"/>
-      <c r="N39" s="7"/>
-      <c r="O39" s="11"/>
-      <c r="P39" s="11"/>
-      <c r="Q39" s="7"/>
-      <c r="R39" s="11"/>
-      <c r="S39" s="11"/>
-      <c r="T39" s="7"/>
-      <c r="U39" s="11"/>
-      <c r="V39" s="11"/>
-      <c r="W39" s="7"/>
-      <c r="X39" s="11"/>
-      <c r="Y39" s="11"/>
-      <c r="Z39" s="7"/>
-      <c r="AA39" s="11"/>
-      <c r="AB39" s="11"/>
-      <c r="AC39" s="7"/>
-      <c r="AD39" s="11"/>
-      <c r="AE39" s="8"/>
-    </row>
-    <row r="40" spans="1:31" x14ac:dyDescent="0.35">
-      <c r="A40" s="16" t="s">
+      <c r="B42" s="7"/>
+      <c r="C42" s="11"/>
+      <c r="D42" s="8"/>
+      <c r="E42" s="7"/>
+      <c r="F42" s="11"/>
+      <c r="G42" s="8"/>
+      <c r="H42" s="7"/>
+      <c r="I42" s="11"/>
+      <c r="J42" s="8"/>
+      <c r="K42" s="7"/>
+      <c r="L42" s="11"/>
+      <c r="M42" s="11"/>
+      <c r="N42" s="7"/>
+      <c r="O42" s="11"/>
+      <c r="P42" s="11"/>
+      <c r="Q42" s="7"/>
+      <c r="R42" s="11"/>
+      <c r="S42" s="11"/>
+      <c r="T42" s="7"/>
+      <c r="U42" s="11"/>
+      <c r="V42" s="11"/>
+      <c r="W42" s="7"/>
+      <c r="X42" s="11"/>
+      <c r="Y42" s="11"/>
+      <c r="Z42" s="7"/>
+      <c r="AA42" s="11"/>
+      <c r="AB42" s="11"/>
+      <c r="AC42" s="7"/>
+      <c r="AD42" s="11"/>
+      <c r="AE42" s="8"/>
+    </row>
+    <row r="43" spans="1:31" x14ac:dyDescent="0.35">
+      <c r="A43" s="15" t="s">
         <v>23</v>
       </c>
-      <c r="B40" s="14">
+      <c r="B43" s="13">
         <v>0.66666666666666596</v>
       </c>
-      <c r="C40" s="15">
+      <c r="C43" s="14">
         <v>0.35294117647058798</v>
       </c>
-      <c r="D40" s="15">
+      <c r="D43" s="14">
         <v>0.85714285714285698</v>
       </c>
-      <c r="E40" s="14">
+      <c r="E43" s="13">
         <v>0.62937062937062904</v>
       </c>
-      <c r="F40" s="15">
+      <c r="F43" s="14">
         <v>0.305084745762711</v>
       </c>
-      <c r="G40" s="15">
+      <c r="G43" s="14">
         <v>0.85714285714285698</v>
       </c>
-      <c r="H40" s="14">
+      <c r="H43" s="13">
         <v>0.66666666666666596</v>
       </c>
-      <c r="I40" s="15">
+      <c r="I43" s="14">
         <v>0.32727272727272699</v>
       </c>
-      <c r="J40" s="15">
+      <c r="J43" s="14">
         <v>0.9</v>
       </c>
-      <c r="K40" s="14">
+      <c r="K43" s="13">
         <v>0.56603773584905603</v>
       </c>
-      <c r="L40" s="15">
+      <c r="L43" s="14">
         <v>0.227848101265822</v>
       </c>
-      <c r="M40" s="15">
+      <c r="M43" s="14">
         <v>0.9</v>
       </c>
-      <c r="N40" s="14">
+      <c r="N43" s="13">
         <v>0.52631578947368396</v>
       </c>
-      <c r="O40" s="15">
+      <c r="O43" s="14">
         <v>0.23529411764705799</v>
       </c>
-      <c r="P40" s="15">
+      <c r="P43" s="14">
         <v>0.76190476190476097</v>
       </c>
-      <c r="Q40" s="14">
+      <c r="Q43" s="13">
         <v>0.6640625</v>
       </c>
-      <c r="R40" s="15">
+      <c r="R43" s="14">
         <v>0.32692307692307598</v>
       </c>
-      <c r="S40" s="15">
+      <c r="S43" s="14">
         <v>0.89473684210526305</v>
       </c>
-      <c r="T40" s="14">
+      <c r="T43" s="13">
         <v>0.68493150684931403</v>
       </c>
-      <c r="U40" s="15">
+      <c r="U43" s="14">
         <v>0.32258064516128998</v>
       </c>
-      <c r="V40" s="15">
+      <c r="V43" s="14">
         <v>0.952380952380952</v>
       </c>
-      <c r="W40" s="14">
+      <c r="W43" s="13">
         <v>0.69277108433734902</v>
       </c>
-      <c r="X40" s="15">
+      <c r="X43" s="14">
         <v>0.34848484848484801</v>
       </c>
-      <c r="Y40" s="15">
+      <c r="Y43" s="14">
         <v>0.92</v>
       </c>
-      <c r="Z40" s="14">
+      <c r="Z43" s="13">
         <v>0.64393939393939303</v>
       </c>
-      <c r="AA40" s="15">
+      <c r="AA43" s="14">
         <v>0.30357142857142799</v>
       </c>
-      <c r="AB40" s="15">
+      <c r="AB43" s="14">
         <v>0.89473684210526305</v>
       </c>
-      <c r="AC40" s="14">
+      <c r="AC43" s="13">
         <v>0.65789473684210498</v>
       </c>
-      <c r="AD40" s="15">
+      <c r="AD43" s="14">
         <v>0.29411764705882298</v>
       </c>
-      <c r="AE40" s="23">
+      <c r="AE43" s="21">
         <v>0.952380952380952</v>
       </c>
-    </row>
-    <row r="41" spans="1:31" x14ac:dyDescent="0.35">
-      <c r="A41" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="B41" s="6">
-        <v>0.49180327868852403</v>
-      </c>
-      <c r="C41" s="10">
-        <v>0.46153846153846101</v>
-      </c>
-      <c r="D41" s="10">
-        <v>0.5</v>
-      </c>
-      <c r="E41" s="6">
-        <v>0.30612244897959101</v>
-      </c>
-      <c r="F41" s="10">
-        <v>0.33333333333333298</v>
-      </c>
-      <c r="G41" s="10">
-        <v>0.3</v>
-      </c>
-      <c r="H41" s="6">
-        <v>0.40983606557377</v>
-      </c>
-      <c r="I41" s="10">
-        <v>0.38461538461538403</v>
-      </c>
-      <c r="J41" s="10">
-        <v>0.41666666666666602</v>
-      </c>
-      <c r="K41" s="6">
-        <v>0.48913043478260798</v>
-      </c>
-      <c r="L41" s="10">
-        <v>0.28125</v>
-      </c>
-      <c r="M41" s="10">
-        <v>0.6</v>
-      </c>
-      <c r="N41" s="6">
-        <v>0.37878787878787801</v>
-      </c>
-      <c r="O41" s="10">
-        <v>0.22727272727272699</v>
-      </c>
-      <c r="P41" s="10">
-        <v>0.45454545454545398</v>
-      </c>
-      <c r="Q41" s="6">
-        <v>0.53571428571428503</v>
-      </c>
-      <c r="R41" s="10">
-        <v>0.5</v>
-      </c>
-      <c r="S41" s="10">
-        <v>0.54545454545454497</v>
-      </c>
-      <c r="T41" s="6">
-        <v>0.390625</v>
-      </c>
-      <c r="U41" s="10">
-        <v>0.3125</v>
-      </c>
-      <c r="V41" s="10">
-        <v>0.41666666666666602</v>
-      </c>
-      <c r="W41" s="6">
-        <v>0.390625</v>
-      </c>
-      <c r="X41" s="10">
-        <v>0.3125</v>
-      </c>
-      <c r="Y41" s="10">
-        <v>0.41666666666666602</v>
-      </c>
-      <c r="Z41" s="6">
-        <v>0.37878787878787801</v>
-      </c>
-      <c r="AA41" s="10">
-        <v>0.27777777777777701</v>
-      </c>
-      <c r="AB41" s="10">
-        <v>0.41666666666666602</v>
-      </c>
-      <c r="AC41" s="6">
-        <v>0.35714285714285698</v>
-      </c>
-      <c r="AD41" s="10">
-        <v>0.25</v>
-      </c>
-      <c r="AE41" s="24">
-        <v>0.4</v>
-      </c>
-    </row>
-    <row r="42" spans="1:31" x14ac:dyDescent="0.35">
-      <c r="A42" s="3"/>
-      <c r="B42" s="6"/>
-      <c r="C42" s="10"/>
-      <c r="D42" s="10"/>
-      <c r="E42" s="6"/>
-      <c r="F42" s="10"/>
-      <c r="G42" s="10"/>
-      <c r="H42" s="6"/>
-      <c r="I42" s="10"/>
-      <c r="J42" s="10"/>
-      <c r="K42" s="6"/>
-      <c r="L42" s="10"/>
-      <c r="M42" s="10"/>
-      <c r="N42" s="6"/>
-      <c r="O42" s="10"/>
-      <c r="P42" s="10"/>
-      <c r="Q42" s="6"/>
-      <c r="R42" s="10"/>
-      <c r="S42" s="10"/>
-      <c r="T42" s="6"/>
-      <c r="U42" s="10"/>
-      <c r="V42" s="10"/>
-      <c r="W42" s="6"/>
-      <c r="X42" s="10"/>
-      <c r="Y42" s="10"/>
-      <c r="Z42" s="6"/>
-      <c r="AA42" s="10"/>
-      <c r="AB42" s="10"/>
-      <c r="AC42" s="6"/>
-      <c r="AD42" s="10"/>
-      <c r="AE42" s="24"/>
-    </row>
-    <row r="43" spans="1:31" x14ac:dyDescent="0.35">
-      <c r="A43" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="B43" s="7"/>
-      <c r="C43" s="11"/>
-      <c r="D43" s="8"/>
-      <c r="E43" s="7"/>
-      <c r="F43" s="11"/>
-      <c r="G43" s="8"/>
-      <c r="H43" s="7"/>
-      <c r="I43" s="11"/>
-      <c r="J43" s="8"/>
-      <c r="K43" s="7"/>
-      <c r="L43" s="11"/>
-      <c r="M43" s="11"/>
-      <c r="N43" s="7"/>
-      <c r="O43" s="11"/>
-      <c r="P43" s="11"/>
-      <c r="Q43" s="7"/>
-      <c r="R43" s="11"/>
-      <c r="S43" s="11"/>
-      <c r="T43" s="7"/>
-      <c r="U43" s="11"/>
-      <c r="V43" s="11"/>
-      <c r="W43" s="7"/>
-      <c r="X43" s="11"/>
-      <c r="Y43" s="11"/>
-      <c r="Z43" s="7"/>
-      <c r="AA43" s="11"/>
-      <c r="AB43" s="11"/>
-      <c r="AC43" s="7"/>
-      <c r="AD43" s="11"/>
-      <c r="AE43" s="8"/>
     </row>
     <row r="44" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A44" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="B44" s="6">
+        <v>0.49180327868852403</v>
+      </c>
+      <c r="C44" s="10">
+        <v>0.46153846153846101</v>
+      </c>
+      <c r="D44" s="10">
+        <v>0.5</v>
+      </c>
+      <c r="E44" s="6">
+        <v>0.30612244897959101</v>
+      </c>
+      <c r="F44" s="10">
+        <v>0.33333333333333298</v>
+      </c>
+      <c r="G44" s="10">
+        <v>0.3</v>
+      </c>
+      <c r="H44" s="6">
+        <v>0.40983606557377</v>
+      </c>
+      <c r="I44" s="10">
+        <v>0.38461538461538403</v>
+      </c>
+      <c r="J44" s="10">
+        <v>0.41666666666666602</v>
+      </c>
+      <c r="K44" s="6">
+        <v>0.48913043478260798</v>
+      </c>
+      <c r="L44" s="10">
+        <v>0.28125</v>
+      </c>
+      <c r="M44" s="10">
+        <v>0.6</v>
+      </c>
+      <c r="N44" s="6">
+        <v>0.37878787878787801</v>
+      </c>
+      <c r="O44" s="10">
+        <v>0.22727272727272699</v>
+      </c>
+      <c r="P44" s="10">
+        <v>0.45454545454545398</v>
+      </c>
+      <c r="Q44" s="6">
+        <v>0.53571428571428503</v>
+      </c>
+      <c r="R44" s="10">
+        <v>0.5</v>
+      </c>
+      <c r="S44" s="10">
+        <v>0.54545454545454497</v>
+      </c>
+      <c r="T44" s="6">
+        <v>0.390625</v>
+      </c>
+      <c r="U44" s="10">
+        <v>0.3125</v>
+      </c>
+      <c r="V44" s="10">
+        <v>0.41666666666666602</v>
+      </c>
+      <c r="W44" s="6">
+        <v>0.390625</v>
+      </c>
+      <c r="X44" s="10">
+        <v>0.3125</v>
+      </c>
+      <c r="Y44" s="10">
+        <v>0.41666666666666602</v>
+      </c>
+      <c r="Z44" s="6">
+        <v>0.37878787878787801</v>
+      </c>
+      <c r="AA44" s="10">
+        <v>0.27777777777777701</v>
+      </c>
+      <c r="AB44" s="10">
+        <v>0.41666666666666602</v>
+      </c>
+      <c r="AC44" s="6">
+        <v>0.35714285714285698</v>
+      </c>
+      <c r="AD44" s="10">
+        <v>0.25</v>
+      </c>
+      <c r="AE44" s="22">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="45" spans="1:31" x14ac:dyDescent="0.35">
+      <c r="A45" s="3"/>
+      <c r="B45" s="6"/>
+      <c r="C45" s="10"/>
+      <c r="D45" s="10"/>
+      <c r="E45" s="6"/>
+      <c r="F45" s="10"/>
+      <c r="G45" s="10"/>
+      <c r="H45" s="6"/>
+      <c r="I45" s="10"/>
+      <c r="J45" s="10"/>
+      <c r="K45" s="6"/>
+      <c r="L45" s="10"/>
+      <c r="M45" s="10"/>
+      <c r="N45" s="6"/>
+      <c r="O45" s="10"/>
+      <c r="P45" s="10"/>
+      <c r="Q45" s="6"/>
+      <c r="R45" s="10"/>
+      <c r="S45" s="10"/>
+      <c r="T45" s="6"/>
+      <c r="U45" s="10"/>
+      <c r="V45" s="10"/>
+      <c r="W45" s="6"/>
+      <c r="X45" s="10"/>
+      <c r="Y45" s="10"/>
+      <c r="Z45" s="6"/>
+      <c r="AA45" s="10"/>
+      <c r="AB45" s="10"/>
+      <c r="AC45" s="6"/>
+      <c r="AD45" s="10"/>
+      <c r="AE45" s="22"/>
+    </row>
+    <row r="46" spans="1:31" x14ac:dyDescent="0.35">
+      <c r="A46" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B46" s="7"/>
+      <c r="C46" s="11"/>
+      <c r="D46" s="8"/>
+      <c r="E46" s="7"/>
+      <c r="F46" s="11"/>
+      <c r="G46" s="8"/>
+      <c r="H46" s="7"/>
+      <c r="I46" s="11"/>
+      <c r="J46" s="8"/>
+      <c r="K46" s="7"/>
+      <c r="L46" s="11"/>
+      <c r="M46" s="11"/>
+      <c r="N46" s="7"/>
+      <c r="O46" s="11"/>
+      <c r="P46" s="11"/>
+      <c r="Q46" s="7"/>
+      <c r="R46" s="11"/>
+      <c r="S46" s="11"/>
+      <c r="T46" s="7"/>
+      <c r="U46" s="11"/>
+      <c r="V46" s="11"/>
+      <c r="W46" s="7"/>
+      <c r="X46" s="11"/>
+      <c r="Y46" s="11"/>
+      <c r="Z46" s="7"/>
+      <c r="AA46" s="11"/>
+      <c r="AB46" s="11"/>
+      <c r="AC46" s="7"/>
+      <c r="AD46" s="11"/>
+      <c r="AE46" s="8"/>
+    </row>
+    <row r="47" spans="1:31" x14ac:dyDescent="0.35">
+      <c r="A47" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="B44" s="6">
+      <c r="B47" s="6">
         <v>0.547445255474452</v>
       </c>
-      <c r="C44" s="10">
+      <c r="C47" s="10">
         <v>0.23076923076923</v>
       </c>
-      <c r="D44" s="10">
+      <c r="D47" s="10">
         <v>0.83333333333333304</v>
       </c>
-      <c r="E44" s="6">
+      <c r="E47" s="6">
         <v>0.52631578947368396</v>
       </c>
-      <c r="F44" s="10">
+      <c r="F47" s="10">
         <v>0.21538461538461501</v>
       </c>
-      <c r="G44" s="10">
+      <c r="G47" s="10">
         <v>0.82352941176470495</v>
       </c>
-      <c r="H44" s="6">
+      <c r="H47" s="6">
         <v>0.53030303030303005</v>
       </c>
-      <c r="I44" s="10">
+      <c r="I47" s="10">
         <v>0.21875</v>
       </c>
-      <c r="J44" s="10">
+      <c r="J47" s="10">
         <v>0.82352941176470495</v>
       </c>
-      <c r="K44" s="6">
+      <c r="K47" s="6">
         <v>0.49242424242424199</v>
       </c>
-      <c r="L44" s="10">
+      <c r="L47" s="10">
         <v>0.191176470588235</v>
       </c>
-      <c r="M44" s="10">
+      <c r="M47" s="10">
         <v>0.8125</v>
       </c>
-      <c r="N44" s="6">
+      <c r="N47" s="6">
         <v>0.59375</v>
       </c>
-      <c r="O44" s="10">
+      <c r="O47" s="10">
         <v>0.26388888888888801</v>
       </c>
-      <c r="P44" s="10">
+      <c r="P47" s="10">
         <v>0.86363636363636298</v>
       </c>
-      <c r="Q44" s="6">
+      <c r="Q47" s="6">
         <v>0.52631578947368396</v>
       </c>
-      <c r="R44" s="10">
+      <c r="R47" s="10">
         <v>0.21538461538461501</v>
       </c>
-      <c r="S44" s="10">
+      <c r="S47" s="10">
         <v>0.82352941176470495</v>
       </c>
-      <c r="T44" s="6">
+      <c r="T47" s="6">
         <v>0.52631578947368396</v>
       </c>
-      <c r="U44" s="10">
+      <c r="U47" s="10">
         <v>0.21538461538461501</v>
       </c>
-      <c r="V44" s="10">
+      <c r="V47" s="10">
         <v>0.82352941176470495</v>
       </c>
-      <c r="W44" s="6">
+      <c r="W47" s="6">
         <v>0.59027777777777701</v>
       </c>
-      <c r="X44" s="10">
+      <c r="X47" s="10">
         <v>0.25</v>
       </c>
-      <c r="Y44" s="10">
+      <c r="Y47" s="10">
         <v>0.89473684210526305</v>
       </c>
-      <c r="Z44" s="6">
+      <c r="Z47" s="6">
         <v>0.48148148148148101</v>
       </c>
-      <c r="AA44" s="10">
+      <c r="AA47" s="10">
         <v>0.194029850746268</v>
       </c>
-      <c r="AB44" s="10">
+      <c r="AB47" s="10">
         <v>0.76470588235294101</v>
       </c>
-      <c r="AC44" s="6">
+      <c r="AC47" s="6">
         <v>0.44</v>
       </c>
-      <c r="AD44" s="10">
+      <c r="AD47" s="10">
         <v>0.16923076923076899</v>
       </c>
-      <c r="AE44" s="24">
+      <c r="AE47" s="22">
         <v>0.73333333333333295</v>
       </c>
     </row>
-    <row r="45" spans="1:31" x14ac:dyDescent="0.35">
-      <c r="A45" s="25" t="s">
+    <row r="48" spans="1:31" x14ac:dyDescent="0.35">
+      <c r="A48" s="23" t="s">
         <v>22</v>
       </c>
-      <c r="B45" s="27">
+      <c r="B48" s="24">
         <v>0.56390977443609003</v>
       </c>
-      <c r="C45" s="28">
+      <c r="C48" s="25">
         <v>0.23076923076923</v>
       </c>
-      <c r="D45" s="28">
+      <c r="D48" s="25">
         <v>0.88235294117647001</v>
       </c>
-      <c r="E45" s="27">
+      <c r="E48" s="24">
         <v>0.495867768595041</v>
       </c>
-      <c r="F45" s="28">
+      <c r="F48" s="25">
         <v>0.18461538461538399</v>
       </c>
-      <c r="G45" s="28">
+      <c r="G48" s="25">
         <v>0.85714285714285698</v>
       </c>
-      <c r="H45" s="27">
+      <c r="H48" s="24">
         <v>0.52419354838709598</v>
       </c>
-      <c r="I45" s="28">
+      <c r="I48" s="25">
         <v>0.203125</v>
       </c>
-      <c r="J45" s="28">
+      <c r="J48" s="25">
         <v>0.86666666666666603</v>
       </c>
-      <c r="K45" s="27">
+      <c r="K48" s="24">
         <v>0.50335570469798596</v>
       </c>
-      <c r="L45" s="28">
+      <c r="L48" s="25">
         <v>0.20547945205479401</v>
       </c>
-      <c r="M45" s="28">
+      <c r="M48" s="25">
         <v>0.78947368421052599</v>
       </c>
-      <c r="N45" s="27">
+      <c r="N48" s="24">
         <v>0.54421768707482998</v>
       </c>
-      <c r="O45" s="28">
+      <c r="O48" s="25">
         <v>0.21333333333333299</v>
       </c>
-      <c r="P45" s="28">
+      <c r="P48" s="25">
         <v>0.88888888888888795</v>
       </c>
-      <c r="Q45" s="27">
+      <c r="Q48" s="24">
         <v>0.57851239669421395</v>
       </c>
-      <c r="R45" s="28">
+      <c r="R48" s="25">
         <v>0.24561403508771901</v>
       </c>
-      <c r="S45" s="28">
+      <c r="S48" s="25">
         <v>0.875</v>
       </c>
-      <c r="T45" s="27">
+      <c r="T48" s="24">
         <v>0.53846153846153799</v>
       </c>
-      <c r="U45" s="28">
+      <c r="U48" s="25">
         <v>0.225806451612903</v>
       </c>
-      <c r="V45" s="28">
+      <c r="V48" s="25">
         <v>0.82352941176470495</v>
       </c>
-      <c r="W45" s="27">
+      <c r="W48" s="24">
         <v>0.625</v>
       </c>
-      <c r="X45" s="28">
+      <c r="X48" s="25">
         <v>0.28125</v>
       </c>
-      <c r="Y45" s="28">
+      <c r="Y48" s="25">
         <v>0.9</v>
       </c>
-      <c r="Z45" s="27">
+      <c r="Z48" s="24">
         <v>0.52083333333333304</v>
       </c>
-      <c r="AA45" s="28">
+      <c r="AA48" s="25">
         <v>0.220588235294117</v>
       </c>
-      <c r="AB45" s="28">
+      <c r="AB48" s="25">
         <v>0.78947368421052599</v>
       </c>
-      <c r="AC45" s="27">
+      <c r="AC48" s="24">
         <v>0.46153846153846101</v>
       </c>
-      <c r="AD45" s="28">
+      <c r="AD48" s="25">
         <v>0.17142857142857101</v>
       </c>
-      <c r="AE45" s="29">
+      <c r="AE48" s="26">
         <v>0.8</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="20">
-    <mergeCell ref="Q20:S20"/>
-    <mergeCell ref="T20:V20"/>
-    <mergeCell ref="W20:Y20"/>
-    <mergeCell ref="Z20:AB20"/>
-    <mergeCell ref="AC20:AE20"/>
-    <mergeCell ref="B20:D20"/>
-    <mergeCell ref="E20:G20"/>
-    <mergeCell ref="H20:J20"/>
-    <mergeCell ref="K20:M20"/>
-    <mergeCell ref="N20:P20"/>
     <mergeCell ref="T4:V4"/>
     <mergeCell ref="W4:Y4"/>
     <mergeCell ref="Z4:AB4"/>
@@ -3999,6 +4166,16 @@
     <mergeCell ref="K4:M4"/>
     <mergeCell ref="N4:P4"/>
     <mergeCell ref="Q4:S4"/>
+    <mergeCell ref="B23:D23"/>
+    <mergeCell ref="E23:G23"/>
+    <mergeCell ref="H23:J23"/>
+    <mergeCell ref="K23:M23"/>
+    <mergeCell ref="N23:P23"/>
+    <mergeCell ref="Q23:S23"/>
+    <mergeCell ref="T23:V23"/>
+    <mergeCell ref="W23:Y23"/>
+    <mergeCell ref="Z23:AB23"/>
+    <mergeCell ref="AC23:AE23"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>